<commit_message>
update schedule with presentation
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A39E482-7100-AE4C-8FA6-71CC0C6D6E88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F79EF9ED-9497-594F-8220-F4CFD7A39031}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="460" windowWidth="35040" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="72">
   <si>
     <t>Topic</t>
   </si>
@@ -303,6 +303,12 @@
   <si>
     <t>- Tufte, pp. xx-xx
 - **Topic and 3 Questions Due**</t>
+  </si>
+  <si>
+    <t>CI: ATE, LATE, TTT</t>
+  </si>
+  <si>
+    <t>7 minute presentations + 7 minutes of questions per group</t>
   </si>
 </sst>
 </file>
@@ -705,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -828,100 +834,103 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="85">
+    <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="34">
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="85">
       <c r="A11" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="136">
+        <v>58</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="34">
       <c r="A12" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="34">
+        <v>16</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="136">
       <c r="A13" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="17">
+        <v>17</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="34">
       <c r="A14" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="204">
+      <c r="B14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="17">
       <c r="A15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>19</v>
+      <c r="B15" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="153">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="204">
       <c r="A16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="372">
+      <c r="B16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="153">
       <c r="A17" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="372">
       <c r="A18" s="2" t="s">
         <v>41</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -979,7 +988,9 @@
       <c r="B26" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="3"/>
+      <c r="C26" s="3" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2" t="s">
@@ -988,7 +999,9 @@
       <c r="B27" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="3"/>
+      <c r="C27" s="3" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2" t="s">
@@ -997,15 +1010,15 @@
       <c r="B28" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C28" s="3"/>
+      <c r="C28" s="3" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>68</v>
-      </c>
+      <c r="B29" s="3"/>
       <c r="C29" s="1"/>
     </row>
     <row r="30" spans="1:4">

</xml_diff>

<commit_message>
add taxonomy of questions, update schedule
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F79EF9ED-9497-594F-8220-F4CFD7A39031}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB49112-B6EA-3644-A3F1-F98AB927F8CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="460" windowWidth="35040" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -69,10 +69,6 @@
     <t>Course Overview</t>
   </si>
   <si>
-    <t>- Read and sign syllabus
-- Submit substantive interest survey</t>
-  </si>
-  <si>
     <t>CI: Potential Outcomes Framework</t>
   </si>
   <si>
@@ -92,9 +88,6 @@
   </si>
   <si>
     <t>CI: Natural Experiments</t>
-  </si>
-  <si>
-    <t>- Descriptive Questions</t>
   </si>
   <si>
     <t>Specifying Counter-Factuals</t>
@@ -233,19 +226,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Angrist and Piscke, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="SFBX1200"/>
-      </rPr>
-      <t xml:space="preserve">Pages 249- 268. </t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Angrist and Piscke </t>
     </r>
     <r>
@@ -273,11 +253,6 @@
 - `Diversity in AI is not your problem, it's hers &lt;https://medium.com/@robert.munro/bias-in-ai-3ea569f79d6a&gt;`_</t>
   </si>
   <si>
-    <t xml:space="preserve">- `Fixed Effects v. Hierarchical Models &lt;fixed_effects_v_hierarchical.ipynb&gt;`_
-- `Interpreting Indicator Vars &lt;interpreting_indicator_vars.ipynb&gt;`_
-</t>
-  </si>
-  <si>
     <t>Converting stakeholder prompts to questions</t>
   </si>
   <si>
@@ -309,6 +284,33 @@
   </si>
   <si>
     <t>7 minute presentations + 7 minutes of questions per group</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- Angrist and Piscke, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="SFBX1200"/>
+      </rPr>
+      <t xml:space="preserve">Pages 249- 268. </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">- `Fixed Effects v. Hierarchical Models &lt;fixed_effects_v_hierarchical.ipynb&gt;`_
+- `Interpreting Indicator Vars &lt;interpreting_indicator_vars.ipynb&gt;`_
+- Callahan, pp. 72-89 
+</t>
+  </si>
+  <si>
+    <t>- `Mere Description &lt;https://doi.org/10.1017/S0007123412000130&gt;`_</t>
+  </si>
+  <si>
+    <t>- Read and sign syllabus
+- Submit substantive interest survey
+- `Taxonomy of Questions &lt;taxonomy_of_questions.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -711,8 +713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -738,7 +740,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>11</v>
@@ -746,15 +748,15 @@
       <c r="C2" s="3"/>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:4" ht="29">
+    <row r="3" spans="1:4" ht="57">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>3</v>
@@ -762,180 +764,180 @@
     </row>
     <row r="4" spans="1:4" ht="17">
       <c r="A4" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="9"/>
     </row>
-    <row r="6" spans="1:4" ht="17">
+    <row r="6" spans="1:4" ht="43">
       <c r="A6" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="29">
       <c r="A7" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="187">
       <c r="A8" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17">
       <c r="A9" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="85">
       <c r="A11" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="34">
       <c r="A12" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="153">
+      <c r="A13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="136">
-      <c r="A13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="C13" s="7" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="34">
       <c r="A14" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17">
       <c r="A15" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="204">
       <c r="A16" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="153">
       <c r="A17" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="372">
       <c r="A18" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
@@ -943,7 +945,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
@@ -952,78 +954,78 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="1"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update with taxonomy of questions
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB49112-B6EA-3644-A3F1-F98AB927F8CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1211A5A-F70D-E44F-9DCE-A7B40696D4DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="460" windowWidth="35040" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="74">
   <si>
     <t>Topic</t>
   </si>
@@ -187,6 +187,111 @@
   </si>
   <si>
     <t>Wed, Apr 15</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Angrist and Piscke, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="SFBX1200"/>
+      </rPr>
+      <t xml:space="preserve">Pages 3-24. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Angrist and Piscke </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="SFBX1200"/>
+      </rPr>
+      <t xml:space="preserve">Pages 222-247. </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">`Matching Methods for Causal Inference: A Review and a Look Forward &lt;https://www.ncbi.nlm.nih.gov/pmc/articles/PMC2943670/&gt;`_ </t>
+  </si>
+  <si>
+    <t>Prediction: ML Bias</t>
+  </si>
+  <si>
+    <t>Prediction: ML versus Casual Inference</t>
+  </si>
+  <si>
+    <t>- `ProPublica: Machine Bias &lt;https://www.propublica.org/article/machine-bias-risk-assessments-in-criminal-sentencing&gt;`_
+- `Racial Bias in Medical Algorithm &lt;https://www.washingtonpost.com/health/2019/10/24/racial-bias-medical-algorithm-favors-white-patients-over-sicker-black-patients/&gt;`_
+- `Amazon scraps secret AI recruiting tool due to bias &lt;https://www.reuters.com/article/us-amazon-com-jobs-automation-insight/amazon-scraps-secret-ai-recruiting-tool-that-showed-bias-against-women-idUSKCN1MK08G&gt;`_
+- `Diversity in AI is not your problem, it's hers &lt;https://medium.com/@robert.munro/bias-in-ai-3ea569f79d6a&gt;`_</t>
+  </si>
+  <si>
+    <t>Converting stakeholder prompts to questions</t>
+  </si>
+  <si>
+    <t>- **Final Project Proposal Due**</t>
+  </si>
+  <si>
+    <t>- **Causal Inference Pset Due**</t>
+  </si>
+  <si>
+    <t>- Dunning (2008). `Improving Causal Inference: Strengths and Limitations of Natural Experiments &lt;http://www.thaddunning.com/wp-content/uploads/2010/03/Dunning_PRQ.pdf&gt;`_
+- 99% Invisible, `Episode 352: Uptown Squirrel. &lt;https://99percentinvisible.org/episode/uptown-squirrel&gt;`_</t>
+  </si>
+  <si>
+    <t>- Fragility
+- Adversarial Users
+- Lucas Critique
+- `Robograders &lt;https://www.vice.com/en_us/article/pa7dj9/flawed-algorithms-are-grading-millions-of-students-essays&gt;`_
+- **Project Proposal Draft Due**</t>
+  </si>
+  <si>
+    <t>Project Presentations</t>
+  </si>
+  <si>
+    <t>CI: ATE, LATE, TTT</t>
+  </si>
+  <si>
+    <t>7 minute presentations + 7 minutes of questions per group</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- Angrist and Piscke, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="SFBX1200"/>
+      </rPr>
+      <t xml:space="preserve">Pages 249- 268. </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">- `Fixed Effects v. Hierarchical Models &lt;fixed_effects_v_hierarchical.ipynb&gt;`_
+- `Interpreting Indicator Vars &lt;interpreting_indicator_vars.ipynb&gt;`_
+- Callahan, pp. 72-89 
+</t>
+  </si>
+  <si>
+    <t>- `Mere Description &lt;https://doi.org/10.1017/S0007123412000130&gt;`_</t>
+  </si>
+  <si>
+    <t>- Read and sign syllabus
+- Submit substantive interest survey
+- `Taxonomy of Questions &lt;taxonomy_of_questions.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- Description and the Problem of Choice
+- Tufte, pp. xx-xx
+- **Topic and 3 Questions Due**</t>
+  </si>
+  <si>
+    <t>CI: Ghost Map</t>
   </si>
   <si>
     <r>
@@ -206,111 +311,12 @@
         <color theme="1"/>
         <rFont val="SFRM1200"/>
       </rPr>
-      <t>. 
-- `The Ghost Map &lt;https://www.amazon.com/Ghost-Map-Londons-Terrifying-Epidemic/dp/1594482691&gt;`_
+      <t xml:space="preserve">. </t>
+    </r>
+  </si>
+  <si>
+    <t>- `The Ghost Map &lt;https://www.amazon.com/Ghost-Map-Londons-Terrifying-Epidemic/dp/1594482691&gt;`_
 - `Causality in the Time of Cholera &lt;https://papers.ssrn.com/sol3/papers.cfm?abstract_id=3262234&gt;`_</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Angrist and Piscke, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="SFBX1200"/>
-      </rPr>
-      <t xml:space="preserve">Pages 3-24. </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Angrist and Piscke </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="SFBX1200"/>
-      </rPr>
-      <t xml:space="preserve">Pages 222-247. </t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">`Matching Methods for Causal Inference: A Review and a Look Forward &lt;https://www.ncbi.nlm.nih.gov/pmc/articles/PMC2943670/&gt;`_ </t>
-  </si>
-  <si>
-    <t>Prediction: ML Bias</t>
-  </si>
-  <si>
-    <t>Prediction: ML versus Casual Inference</t>
-  </si>
-  <si>
-    <t>- `ProPublica: Machine Bias &lt;https://www.propublica.org/article/machine-bias-risk-assessments-in-criminal-sentencing&gt;`_
-- `Racial Bias in Medical Algorithm &lt;https://www.washingtonpost.com/health/2019/10/24/racial-bias-medical-algorithm-favors-white-patients-over-sicker-black-patients/&gt;`_
-- `Amazon scraps secret AI recruiting tool due to bias &lt;https://www.reuters.com/article/us-amazon-com-jobs-automation-insight/amazon-scraps-secret-ai-recruiting-tool-that-showed-bias-against-women-idUSKCN1MK08G&gt;`_
-- `Diversity in AI is not your problem, it's hers &lt;https://medium.com/@robert.munro/bias-in-ai-3ea569f79d6a&gt;`_</t>
-  </si>
-  <si>
-    <t>Converting stakeholder prompts to questions</t>
-  </si>
-  <si>
-    <t>- **Final Project Proposal Due**</t>
-  </si>
-  <si>
-    <t>- **Causal Inference Pset Due**</t>
-  </si>
-  <si>
-    <t>- Dunning (2008). `Improving Causal Inference: Strengths and Limitations of Natural Experiments &lt;http://www.thaddunning.com/wp-content/uploads/2010/03/Dunning_PRQ.pdf&gt;`_
-- 99% Invisible, `Episode 352: Uptown Squirrel. &lt;https://99percentinvisible.org/episode/uptown-squirrel&gt;`_</t>
-  </si>
-  <si>
-    <t>- Fragility
-- Adversarial Users
-- Lucas Critique
-- `Robograders &lt;https://www.vice.com/en_us/article/pa7dj9/flawed-algorithms-are-grading-millions-of-students-essays&gt;`_
-- **Project Proposal Draft Due**</t>
-  </si>
-  <si>
-    <t>Project Presentations</t>
-  </si>
-  <si>
-    <t>- Tufte, pp. xx-xx
-- **Topic and 3 Questions Due**</t>
-  </si>
-  <si>
-    <t>CI: ATE, LATE, TTT</t>
-  </si>
-  <si>
-    <t>7 minute presentations + 7 minutes of questions per group</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">- Angrist and Piscke, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="SFBX1200"/>
-      </rPr>
-      <t xml:space="preserve">Pages 249- 268. </t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">- `Fixed Effects v. Hierarchical Models &lt;fixed_effects_v_hierarchical.ipynb&gt;`_
-- `Interpreting Indicator Vars &lt;interpreting_indicator_vars.ipynb&gt;`_
-- Callahan, pp. 72-89 
-</t>
-  </si>
-  <si>
-    <t>- `Mere Description &lt;https://doi.org/10.1017/S0007123412000130&gt;`_</t>
-  </si>
-  <si>
-    <t>- Read and sign syllabus
-- Submit substantive interest survey
-- `Taxonomy of Questions &lt;taxonomy_of_questions.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -713,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -756,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>3</v>
@@ -771,7 +777,7 @@
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -791,13 +797,13 @@
         <v>8</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="29">
+    <row r="7" spans="1:4" ht="57">
       <c r="A7" s="2" t="s">
         <v>28</v>
       </c>
@@ -805,13 +811,13 @@
         <v>8</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="187">
+    <row r="8" spans="1:4" ht="34">
       <c r="A8" s="2" t="s">
         <v>29</v>
       </c>
@@ -819,112 +825,112 @@
         <v>12</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="17">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="119">
       <c r="A9" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>71</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="17">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="85">
+        <v>13</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="34">
+      <c r="B11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="85">
       <c r="A12" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="153">
+        <v>14</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="34">
       <c r="A13" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="34">
+        <v>15</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="153">
       <c r="A14" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="17">
+        <v>16</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="34">
       <c r="A15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="204">
+      <c r="B15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="17">
       <c r="A16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>18</v>
+      <c r="B16" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="153">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="204">
       <c r="A17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="372">
+      <c r="B17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="153">
       <c r="A18" s="2" t="s">
         <v>39</v>
       </c>
@@ -932,7 +938,7 @@
         <v>56</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -952,9 +958,15 @@
       </c>
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" ht="372">
       <c r="A21" s="2" t="s">
         <v>42</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -963,7 +975,7 @@
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -988,10 +1000,10 @@
         <v>47</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -999,10 +1011,10 @@
         <v>48</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1010,10 +1022,10 @@
         <v>49</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:4">

</xml_diff>

<commit_message>
substantial updates to class chedule, taxonomy of questions, etc.
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1211A5A-F70D-E44F-9DCE-A7B40696D4DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725C7261-EE24-644D-83AA-5A3808A64E91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="460" windowWidth="35040" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -281,11 +281,6 @@
     <t>- `Mere Description &lt;https://doi.org/10.1017/S0007123412000130&gt;`_</t>
   </si>
   <si>
-    <t>- Read and sign syllabus
-- Submit substantive interest survey
-- `Taxonomy of Questions &lt;taxonomy_of_questions.ipynb&gt;`_</t>
-  </si>
-  <si>
     <t>- Description and the Problem of Choice
 - Tufte, pp. xx-xx
 - **Topic and 3 Questions Due**</t>
@@ -317,6 +312,11 @@
   <si>
     <t>- `The Ghost Map &lt;https://www.amazon.com/Ghost-Map-Londons-Terrifying-Epidemic/dp/1594482691&gt;`_
 - `Causality in the Time of Cholera &lt;https://papers.ssrn.com/sol3/papers.cfm?abstract_id=3262234&gt;`_</t>
+  </si>
+  <si>
+    <t>- Read, sign, submit syllabus. 
+- `Submit substantive interest survey &lt;https://forms.gle/cpr9SB4d7unXRx3j6&gt;`_
+- Read `Taxonomy of Questions &lt;taxonomy_of_questions.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -719,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -754,7 +754,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:4" ht="57">
+    <row r="3" spans="1:4" ht="85">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>3</v>
@@ -811,7 +811,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>22</v>
@@ -825,7 +825,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="119">
@@ -833,10 +833,10 @@
         <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17">

</xml_diff>

<commit_message>
update syllabus with stakeholder interpretation questions
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725C7261-EE24-644D-83AA-5A3808A64E91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02B2E6A-63D1-6F42-8953-3D7DAB00CBAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="460" windowWidth="35040" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="5020" yWindow="7740" windowWidth="35040" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="75">
   <si>
     <t>Topic</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>In-Class Exercise</t>
-  </si>
-  <si>
-    <t>Taxonomy of questions</t>
   </si>
   <si>
     <t>Date</t>
@@ -317,6 +314,12 @@
     <t>- Read, sign, submit syllabus. 
 - `Submit substantive interest survey &lt;https://forms.gle/cpr9SB4d7unXRx3j6&gt;`_
 - Read `Taxonomy of Questions &lt;taxonomy_of_questions.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>Generating Questions</t>
+  </si>
+  <si>
+    <t>- `Moving from Problems to Questions &lt;moving_from_problems_to_questions&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -375,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -403,6 +406,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -720,7 +724,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -732,7 +736,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -746,298 +750,300 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:4" ht="85">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17">
       <c r="A4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="12"/>
+        <v>8</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="D4" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="9"/>
     </row>
     <row r="6" spans="1:4" ht="43">
       <c r="A6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="57">
       <c r="A7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="34">
       <c r="A8" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="119">
       <c r="A9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17">
       <c r="A10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="85">
       <c r="A12" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="34">
       <c r="A13" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="153">
       <c r="A14" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="34">
       <c r="A15" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17">
       <c r="A16" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="204">
       <c r="A17" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="153">
       <c r="A18" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D20" s="8"/>
     </row>
     <row r="21" spans="1:4" ht="372">
       <c r="A21" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="1"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add exercises for wednesday
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1211408F-E083-FF41-A83A-1583ACEACA4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844C7126-392C-B547-9A6D-25D9437FBE01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="580" windowWidth="35040" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="10920" yWindow="460" windowWidth="35040" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule_xlsx" sheetId="1" r:id="rId1"/>
@@ -93,9 +93,6 @@
     <t>Specifying Ideal Experiments</t>
   </si>
   <si>
-    <t>- Exercises</t>
-  </si>
-  <si>
     <t>- Plotting / Choice Parameter Exercises</t>
   </si>
   <si>
@@ -321,6 +318,9 @@
   <si>
     <t>- `Discretion in Descriptive Analyses &lt;descriptive_questions.ipynb&gt;`_
 - `Positive versus Normative Questions &lt;https://www.youtube.com/watch?v=YtX6SGw7E3c&gt;`_</t>
+  </si>
+  <si>
+    <t>`Link &lt;exercises/exercise_descriptive.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -725,7 +725,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -751,7 +751,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>10</v>
@@ -761,35 +761,35 @@
     </row>
     <row r="3" spans="1:4" ht="85">
       <c r="A3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="34">
       <c r="A4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>4</v>
@@ -798,63 +798,63 @@
     </row>
     <row r="6" spans="1:4" ht="85">
       <c r="A6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>74</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="43">
       <c r="A7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="34">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="119">
       <c r="A9" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17">
       <c r="A10" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>18</v>
@@ -862,21 +862,21 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="85">
       <c r="A12" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>19</v>
@@ -884,73 +884,73 @@
     </row>
     <row r="13" spans="1:4" ht="34">
       <c r="A13" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="153">
       <c r="A14" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="34">
       <c r="A15" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17">
       <c r="A16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="204">
       <c r="A17" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="153">
       <c r="A18" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
@@ -958,7 +958,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
@@ -967,84 +967,84 @@
     </row>
     <row r="21" spans="1:4" ht="372">
       <c r="A21" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="1"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update schedule, add counterfactual exercises
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4C58EB-5F42-2E4F-8A38-8FF17AAC3685}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEBF8474-9B5C-5647-AA28-818FA83D43E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="460" windowWidth="35040" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="3960" yWindow="640" windowWidth="35040" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule_xlsx" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="73">
   <si>
     <t>Topic</t>
   </si>
@@ -87,12 +87,6 @@
     <t>CI: Natural Experiments</t>
   </si>
   <si>
-    <t>Specifying Counter-Factuals</t>
-  </si>
-  <si>
-    <t>Specifying Ideal Experiments</t>
-  </si>
-  <si>
     <t>Wed, Jan 8</t>
   </si>
   <si>
@@ -178,19 +172,6 @@
   </si>
   <si>
     <t>Wed, Apr 15</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Angrist and Piscke, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="SFBX1200"/>
-      </rPr>
-      <t xml:space="preserve">Pages 3-24. </t>
-    </r>
   </si>
   <si>
     <r>
@@ -247,8 +228,32 @@
     <t>7 minute presentations + 7 minutes of questions per group</t>
   </si>
   <si>
+    <t>CI: Ghost Map</t>
+  </si>
+  <si>
+    <t>- Read, sign, submit syllabus. 
+- `Submit substantive interest survey &lt;https://forms.gle/cpr9SB4d7unXRx3j6&gt;`_
+- Read `Taxonomy of Questions &lt;taxonomy_of_questions.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Moving from Problems to Questions &lt;moving_from_problems_to_questions&gt;`_</t>
+  </si>
+  <si>
+    <t>`Types of Questions &lt;exercises/exercise_taxonomy_of_questions.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>`Converting stakeholder prompts to questions &lt;exercises/exercise_generating_questions.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Discretion in Descriptive Analyses &lt;descriptive_questions.ipynb&gt;`_
+- `Positive versus Normative Questions &lt;https://www.youtube.com/watch?v=YtX6SGw7E3c&gt;`_</t>
+  </si>
+  <si>
+    <t>`Link &lt;exercises/exercise_descriptive.ipynb&gt;`_</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">- Angrist and Piscke, </t>
+      <t>Angrist and Piscke (MHE) Chapter 1 (p</t>
     </r>
     <r>
       <rPr>
@@ -256,42 +261,12 @@
         <color theme="1"/>
         <rFont val="SFBX1200"/>
       </rPr>
-      <t xml:space="preserve">Pages 249- 268. </t>
+      <t>ages 3-24)</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">- `Fixed Effects v. Hierarchical Models &lt;fixed_effects_v_hierarchical.ipynb&gt;`_
-- `Interpreting Indicator Vars &lt;interpreting_indicator_vars.ipynb&gt;`_
-- Callahan, pp. 72-89 
-</t>
-  </si>
-  <si>
-    <t>CI: Ghost Map</t>
-  </si>
-  <si>
-    <t>- Read, sign, submit syllabus. 
-- `Submit substantive interest survey &lt;https://forms.gle/cpr9SB4d7unXRx3j6&gt;`_
-- Read `Taxonomy of Questions &lt;taxonomy_of_questions.ipynb&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Moving from Problems to Questions &lt;moving_from_problems_to_questions&gt;`_</t>
-  </si>
-  <si>
-    <t>`Types of Questions &lt;exercises/exercise_taxonomy_of_questions.ipynb&gt;`_</t>
-  </si>
-  <si>
-    <t>`Converting stakeholder prompts to questions &lt;exercises/exercise_generating_questions.ipynb&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Discretion in Descriptive Analyses &lt;descriptive_questions.ipynb&gt;`_
-- `Positive versus Normative Questions &lt;https://www.youtube.com/watch?v=YtX6SGw7E3c&gt;`_</t>
-  </si>
-  <si>
-    <t>`Link &lt;exercises/exercise_descriptive.ipynb&gt;`_</t>
-  </si>
-  <si>
     <r>
-      <t xml:space="preserve">- Morgan and Winship. </t>
+      <t xml:space="preserve"> Angrist and Piscke (MM), </t>
     </r>
     <r>
       <rPr>
@@ -299,7 +274,24 @@
         <color theme="1"/>
         <rFont val="SFBX1200"/>
       </rPr>
-      <t>Pages 37-58</t>
+      <t>Pages xi - 32
+(Skip appendix)</t>
+    </r>
+  </si>
+  <si>
+    <t>- `The Ghost Map &lt;https://www.amazon.com/Ghost-Map-Londons-Terrifying-Epidemic/dp/1594482691&gt;`_ pp. 25-54, 111-230</t>
+  </si>
+  <si>
+    <r>
+      <t>- Morgan and Winship. Chapter 1 (p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="SFBX1200"/>
+      </rPr>
+      <t>ages 3-22)</t>
     </r>
     <r>
       <rPr>
@@ -307,13 +299,32 @@
         <color theme="1"/>
         <rFont val="SFRM1200"/>
       </rPr>
-      <t>.</t>
+      <t>.
+- **Topic and 3 Questions Due**</t>
     </r>
   </si>
   <si>
-    <t>- `The Ghost Map &lt;https://www.amazon.com/Ghost-Map-Londons-Terrifying-Epidemic/dp/1594482691&gt;`_
-- `Causality in the Time of Cholera &lt;https://papers.ssrn.com/sol3/papers.cfm?abstract_id=3262234&gt;`_
-- **Topic and 3 Questions Due**</t>
+    <t>`Link &lt;exercises/exercise_counterfactuals.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <r>
+      <t>- Angrist and Piscke (MM), Chapter 2 (pp. 47-82)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="SFBX1200"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">- `Fixed Effects v. Hierarchical Models &lt;fixed_effects_v_hierarchical.ipynb&gt;`_
+-  Kennedy, Sections 18.1-18.3
+- `Interpreting Indicator Vars &lt;interpreting_indicator_vars.ipynb&gt;`_
+- Callahan, pp. 72-89 
+</t>
   </si>
 </sst>
 </file>
@@ -717,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -744,7 +755,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>10</v>
@@ -754,35 +765,35 @@
     </row>
     <row r="3" spans="1:4" ht="85">
       <c r="A3" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="34">
       <c r="A4" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>4</v>
@@ -791,150 +802,153 @@
     </row>
     <row r="6" spans="1:4" ht="85">
       <c r="A6" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="34">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="51">
       <c r="A7" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="51">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="85">
+      <c r="A9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="34">
+      <c r="A10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="85">
+      <c r="A12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="34">
+      <c r="A13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="136">
-      <c r="A8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C8" s="7" t="s">
+    <row r="14" spans="1:4" ht="170">
+      <c r="A14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="17">
-      <c r="A9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="85">
-      <c r="A11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="34">
-      <c r="A12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="153">
-      <c r="A13" s="2" t="s">
+    <row r="15" spans="1:4" ht="34">
+      <c r="A15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="34">
-      <c r="A14" s="2" t="s">
+      <c r="B15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="17">
+      <c r="A16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="10" t="s">
+      <c r="B16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="204">
+      <c r="A17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="153">
+      <c r="A18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="17">
-      <c r="A15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="204">
-      <c r="A16" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="153">
-      <c r="A17" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="2" t="s">
-        <v>36</v>
+      <c r="C18" s="7" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
@@ -942,7 +956,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
@@ -951,84 +965,84 @@
     </row>
     <row r="21" spans="1:4" ht="372">
       <c r="A21" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="1"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update topics deadline and schedule
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3010DEC9-F291-294D-B91E-A00613ED391D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C4D553-288E-734D-9B34-1477BAFAC0EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2720" yWindow="460" windowWidth="35040" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="74">
   <si>
     <t>Topic</t>
   </si>
@@ -336,9 +336,6 @@
       <t xml:space="preserve">
 - `Read first homework &lt;https://github.com/nickeubank/unifyingdatascience/blob/master/project/UDS_Topics_And_Questions/UDS_Topics_And_Questions.pdf&gt;`_</t>
     </r>
-  </si>
-  <si>
-    <t>add think of selection problem</t>
   </si>
 </sst>
 </file>
@@ -743,7 +740,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -838,9 +835,6 @@
       <c r="C7" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>74</v>
-      </c>
     </row>
     <row r="8" spans="1:4" ht="51">
       <c r="A8" s="2" t="s">

</xml_diff>

<commit_message>
add potential outcome notes
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C4D553-288E-734D-9B34-1477BAFAC0EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF08B4B-25F5-374A-B551-4AC978969674}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2720" yWindow="460" windowWidth="35040" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -249,42 +249,7 @@
     <t>`Link &lt;exercises/exercise_descriptive.ipynb&gt;`_</t>
   </si>
   <si>
-    <r>
-      <t>Angrist and Piscke (MHE) Chapter 1 (p</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="SFBX1200"/>
-      </rPr>
-      <t>ages 3-24)</t>
-    </r>
-  </si>
-  <si>
     <t>- `The Ghost Map &lt;https://www.amazon.com/Ghost-Map-Londons-Terrifying-Epidemic/dp/1594482691&gt;`_ pp. 25-54, 111-230</t>
-  </si>
-  <si>
-    <r>
-      <t>- Morgan and Winship. Chapter 1 (p</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="SFBX1200"/>
-      </rPr>
-      <t>ages 3-22)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="SFRM1200"/>
-      </rPr>
-      <t>.
-- **Topic and 3 Questions Due**</t>
-    </r>
   </si>
   <si>
     <t>`Link &lt;exercises/exercise_counterfactuals.ipynb&gt;`_</t>
@@ -335,6 +300,50 @@
       </rPr>
       <t xml:space="preserve">
 - `Read first homework &lt;https://github.com/nickeubank/unifyingdatascience/blob/master/project/UDS_Topics_And_Questions/UDS_Topics_And_Questions.pdf&gt;`_</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>- Angrist and Piscke (MHE) Chapter 1 (p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="SFBX1200"/>
+      </rPr>
+      <t>ages 3-24)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="SFRM1200"/>
+      </rPr>
+      <t xml:space="preserve">
+- **Topic and 3 Questions Due**</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>- Imbens and Rubin. Chapter 1 (p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="SFBX1200"/>
+      </rPr>
+      <t>ages 3-22)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="SFRM1200"/>
+      </rPr>
+      <t>.
+(PDF on Sakai for Duke students)</t>
     </r>
   </si>
 </sst>
@@ -739,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -833,10 +842,10 @@
         <v>11</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="51">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="68">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
@@ -844,10 +853,10 @@
         <v>11</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="85">
@@ -858,18 +867,18 @@
         <v>58</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="34">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="51">
       <c r="A10" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>65</v>
+      <c r="C10" s="11" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -877,10 +886,10 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="85">
@@ -902,7 +911,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="170">
@@ -913,7 +922,7 @@
         <v>15</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="34">

</xml_diff>

<commit_message>
limitations of ATE, update schedule
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D17DC29A-AA99-B641-AF46-C76E9251CAEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B3F26D-40F8-BF40-9580-E4B02A2888F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2180" yWindow="3820" windowWidth="35040" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="2180" yWindow="640" windowWidth="35040" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -78,9 +78,6 @@
     <t>CI: Regression</t>
   </si>
   <si>
-    <t>CI: Fixed Effects</t>
-  </si>
-  <si>
     <t>CI: Difference-in-Differences</t>
   </si>
   <si>
@@ -196,12 +193,6 @@
     <t>Prediction: ML versus Casual Inference</t>
   </si>
   <si>
-    <t>- `ProPublica: Machine Bias &lt;https://www.propublica.org/article/machine-bias-risk-assessments-in-criminal-sentencing&gt;`_
-- `Racial Bias in Medical Algorithm &lt;https://www.washingtonpost.com/health/2019/10/24/racial-bias-medical-algorithm-favors-white-patients-over-sicker-black-patients/&gt;`_
-- `Amazon scraps secret AI recruiting tool due to bias &lt;https://www.reuters.com/article/us-amazon-com-jobs-automation-insight/amazon-scraps-secret-ai-recruiting-tool-that-showed-bias-against-women-idUSKCN1MK08G&gt;`_
-- `Diversity in AI is not your problem, it's hers &lt;https://medium.com/@robert.munro/bias-in-ai-3ea569f79d6a&gt;`_</t>
-  </si>
-  <si>
     <t>- **Final Project Proposal Due**</t>
   </si>
   <si>
@@ -263,13 +254,6 @@
       </rPr>
       <t xml:space="preserve">. </t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">- `Fixed Effects v. Hierarchical Models &lt;fixed_effects_v_hierarchical.ipynb&gt;`_
--  Kennedy, Sections 18.1-18.3
-- `Interpreting Indicator Vars &lt;interpreting_indicator_vars.ipynb&gt;`_
-- Callahan, pp. 72-89 
-</t>
   </si>
   <si>
     <r>
@@ -303,15 +287,26 @@
     <t>Ghost map exercises</t>
   </si>
   <si>
-    <t>Limitations of ATE Concept</t>
-  </si>
-  <si>
     <t xml:space="preserve">- `Moving from Problems to Questions &lt;moving_from_problems_to_questions&gt;`_
 - `Why It's Important To Get Your Question Right &lt;https://www.youtube.com/watch?v=kYMfE9u-lMo&gt;`_
 </t>
   </si>
   <si>
     <t>`Potential Outcome Slides &lt;https://github.com/nickeubank/unifyingdatascience/blob/master/lecture_slides/20_PotentialOutcomes/Eubank_UDS_PotentialOutcomes_Handout.pdf&gt;`_</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - `Limitations of Average Treatment Effects &lt;limitations_of_ATE.ipynb&gt;`_
+- **Topic and 3 Questions Due**</t>
+  </si>
+  <si>
+    <t>CI: LATE / Compliance</t>
+  </si>
+  <si>
+    <t>- `ProPublica: Machine Bias &lt;https://www.propublica.org/article/machine-bias-risk-assessments-in-criminal-sentencing&gt;`_
+- `Racial Bias in Medical Algorithm &lt;https://www.washingtonpost.com/health/2019/10/24/racial-bias-medical-algorithm-favors-white-patients-over-sicker-black-patients/&gt;`_
+- `Amazon scraps secret AI recruiting tool due to bias &lt;https://www.reuters.com/article/us-amazon-com-jobs-automation-insight/amazon-scraps-secret-ai-recruiting-tool-that-showed-bias-against-women-idUSKCN1MK08G&gt;`_
+- `Diversity in AI is not your problem, it's hers &lt;https://medium.com/@robert.munro/bias-in-ai-3ea569f79d6a&gt;`_
+- `Not all AI bias is unintentional... &lt;https://www.washingtonpost.com/nation/2020/01/28/opioid-kickback-software/&gt;`_</t>
   </si>
   <si>
     <r>
@@ -325,13 +320,26 @@
       </rPr>
       <t>ages 3-24)</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve"> - `Limitations of Average Treatment Effects &lt;limitations_of_ATE.ipynb&gt;`_
-- **Topic and 3 Questions Due**</t>
-  </si>
-  <si>
-    <t>CI: LATE / Compliance</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="SFRM1200"/>
+      </rPr>
+      <t xml:space="preserve">
+- Review linear regression in Python (`WM Chapter &lt;https://www.amazon.com/Python-Data-Analysis-Wrangling-IPython-ebook/dp/B075X4LT6K&gt;`_ 13, 13.1, 13.2, 13.3)</t>
+    </r>
+  </si>
+  <si>
+    <t>CI: Fixed Effects and Clustering</t>
+  </si>
+  <si>
+    <t>- `Fixed Effects v. Hierarchical Models &lt;fixed_effects_v_hierarchical.ipynb&gt;`_
+-  Kennedy, Sections 18.1-18.3
+- `Interpreting Indicator Vars &lt;interpreting_indicator_vars.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- Limitations of Experiments and ATE</t>
   </si>
 </sst>
 </file>
@@ -737,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -764,7 +772,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>10</v>
@@ -774,35 +782,35 @@
     </row>
     <row r="3" spans="1:4" ht="85">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="153">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>4</v>
@@ -811,165 +819,165 @@
     </row>
     <row r="6" spans="1:4" ht="85">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="136">
       <c r="A7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="119">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="34">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="153">
       <c r="A9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="68">
       <c r="A10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" t="s">
-        <v>72</v>
+        <v>25</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>77</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="85">
       <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="34">
+      <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C11" s="7" t="s">
+      <c r="B12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="85">
-      <c r="A12" s="2" t="s">
+    </row>
+    <row r="13" spans="1:4" ht="136">
+      <c r="A13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B13" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="85">
+      <c r="A14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="34">
-      <c r="A13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="170">
-      <c r="A14" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>67</v>
+      <c r="C14" s="10" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="34">
       <c r="A15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="204">
       <c r="A17" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
@@ -977,7 +985,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
@@ -986,90 +994,90 @@
     </row>
     <row r="21" spans="1:4" ht="153">
       <c r="A21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="409.6">
+      <c r="A22" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="372">
-      <c r="A22" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="B22" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="1"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add resume exercise preliminaries
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F3A43B-1B02-3B4D-A7E8-0F56702123A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67828F33-9F88-AE4A-B947-A589E6AF4686}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2180" yWindow="640" windowWidth="35040" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="2180" yWindow="620" windowWidth="35040" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -281,9 +281,6 @@
     <t>- `Potential Outcomes &lt;https://www.dropbox.com/s/l85ci4au234jtff/Causal_inference_Materials.zip?dl=0&amp;file_subpath=%2FCausal_inference_Materials%2FPotential_Outcomes.pdf&gt;`_</t>
   </si>
   <si>
-    <t>Experimental Analysis Exercise</t>
-  </si>
-  <si>
     <t>Ghost map exercises</t>
   </si>
   <si>
@@ -343,6 +340,9 @@
       <t xml:space="preserve">
 - Review linear regression in Python (`WM Chapter &lt;https://www.amazon.com/Python-Data-Analysis-Wrangling-IPython-ebook/dp/B075X4LT6K&gt;`_ 13, 13.1, 13.2, 13.3)</t>
     </r>
+  </si>
+  <si>
+    <t>`Link &lt;exercises/exercise_resume.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -749,7 +749,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -805,7 +805,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>59</v>
@@ -845,7 +845,7 @@
         <v>65</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="119">
@@ -870,10 +870,10 @@
         <v>12</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="68">
@@ -881,13 +881,13 @@
         <v>25</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="85">
@@ -901,7 +901,7 @@
         <v>62</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="34">
@@ -920,10 +920,10 @@
         <v>28</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>74</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="85">
@@ -975,7 +975,7 @@
         <v>33</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1014,7 +1014,7 @@
         <v>48</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:4">

</xml_diff>

<commit_message>
update schedules for missing day
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBE3BCA-14BC-B84A-9F0B-1179DCD7C298}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C86D3E8-DBB0-2741-A702-C1EA0C4475E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2180" yWindow="620" windowWidth="35040" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -289,9 +289,6 @@
     <t>`Potential Outcome Slides &lt;https://github.com/nickeubank/unifyingdatascience/blob/master/lecture_slides/20_PotentialOutcomes/Eubank_UDS_PotentialOutcomes_Handout.pdf&gt;`_</t>
   </si>
   <si>
-    <t>CI: LATE / Compliance</t>
-  </si>
-  <si>
     <t>- `ProPublica: Machine Bias &lt;https://www.propublica.org/article/machine-bias-risk-assessments-in-criminal-sentencing&gt;`_
 - `Racial Bias in Medical Algorithm &lt;https://www.washingtonpost.com/health/2019/10/24/racial-bias-medical-algorithm-favors-white-patients-over-sicker-black-patients/&gt;`_
 - `Amazon scraps secret AI recruiting tool due to bias &lt;https://www.reuters.com/article/us-amazon-com-jobs-automation-insight/amazon-scraps-secret-ai-recruiting-tool-that-showed-bias-against-women-idUSKCN1MK08G&gt;`_
@@ -344,6 +341,9 @@
   <si>
     <t>`Link 1 &lt;exercises/exercise_ghostmap_1.ipynb&gt;`_
 `Link 2 &lt;exercises/exercise_ghostmap_2.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>A/B Testing Practicalities</t>
   </si>
 </sst>
 </file>
@@ -749,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -871,10 +871,10 @@
         <v>12</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="68">
@@ -882,13 +882,13 @@
         <v>25</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="85">
@@ -902,81 +902,79 @@
         <v>62</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="34">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="136">
+    </row>
+    <row r="13" spans="1:4" ht="34">
       <c r="A13" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="85">
+        <v>14</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="136">
       <c r="A14" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="34">
+        <v>70</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="85">
       <c r="A15" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="17">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="34">
       <c r="A16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="204">
+      <c r="B16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="17">
       <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>16</v>
+      <c r="B17" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>51</v>
+      </c>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" ht="204">
       <c r="A18" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>69</v>
+        <v>16</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -996,34 +994,36 @@
       </c>
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="1:4" ht="153">
+    <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="409.6">
+      <c r="B21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="153">
       <c r="A22" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="409.6">
       <c r="A23" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="8" t="s">
+      <c r="B23" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add FE exercises and indicator vars
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D6C7957-3649-6441-84B1-C7112813F803}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A22BA555-CE2B-914A-8906-ED162A7F2A20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="580" windowWidth="35040" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="2320" yWindow="6600" windowWidth="35040" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="80">
   <si>
     <t>Topic</t>
   </si>
@@ -344,6 +344,10 @@
       </rPr>
       <t xml:space="preserve"> 178-208) </t>
     </r>
+  </si>
+  <si>
+    <t>- `Indicators &lt;exercises/exercise_indicators.ipynb&gt;`_
+- `Fixed Effects &lt;exercises/exercise_panel.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -750,7 +754,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -935,6 +939,9 @@
       <c r="C14" s="7" t="s">
         <v>77</v>
       </c>
+      <c r="D14" s="7" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="68">
       <c r="A15" s="2" t="s">

</xml_diff>

<commit_message>
add backwards design and update readings
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4768279E-2688-434A-AA63-34D2FD420AE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5052800F-7A4C-7744-9A17-A79BACD4C03B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2320" yWindow="660" windowWidth="35040" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="6340" yWindow="620" windowWidth="35040" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -183,10 +183,6 @@
     <t>- **Final Project Proposal Due**</t>
   </si>
   <si>
-    <t>- Dunning (2008). `Improving Causal Inference: Strengths and Limitations of Natural Experiments &lt;http://www.thaddunning.com/wp-content/uploads/2010/03/Dunning_PRQ.pdf&gt;`_
-- 99% Invisible, `Episode 352: Uptown Squirrel. &lt;https://99percentinvisible.org/episode/uptown-squirrel&gt;`_</t>
-  </si>
-  <si>
     <t>- Fragility
 - Adversarial Users
 - Lucas Critique
@@ -355,6 +351,10 @@
   </si>
   <si>
     <t>- `Link &lt;exercises/exercise_diffindiff.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Angrist and Pischke (MM), Chapter 3 (pp 98-146)
+- Come prepared to discuss backwards design of your group project. </t>
   </si>
 </sst>
 </file>
@@ -760,8 +760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -804,10 +804,10 @@
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="85">
@@ -818,10 +818,10 @@
         <v>8</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -841,10 +841,10 @@
         <v>7</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>58</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="85">
@@ -855,10 +855,10 @@
         <v>11</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="85">
@@ -869,10 +869,10 @@
         <v>11</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="85">
@@ -883,10 +883,10 @@
         <v>12</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="51">
@@ -894,13 +894,13 @@
         <v>25</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="51">
@@ -908,13 +908,13 @@
         <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -930,10 +930,10 @@
         <v>14</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="85">
@@ -941,13 +941,13 @@
         <v>29</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="68">
@@ -961,7 +961,7 @@
         <v>46</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17">
@@ -972,10 +972,10 @@
         <v>15</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17">
@@ -988,7 +988,7 @@
       <c r="C17" s="11"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" ht="119">
+    <row r="18" spans="1:4" ht="51">
       <c r="A18" s="2" t="s">
         <v>33</v>
       </c>
@@ -996,7 +996,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>50</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1021,7 +1021,7 @@
         <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="119">
@@ -1032,7 +1032,7 @@
         <v>48</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="306">
@@ -1043,7 +1043,7 @@
         <v>47</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>49</v>
@@ -1066,10 +1066,10 @@
         <v>41</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1077,10 +1077,10 @@
         <v>42</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1088,10 +1088,10 @@
         <v>43</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:4">

</xml_diff>

<commit_message>
add backwards assignment to syllabus
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5052800F-7A4C-7744-9A17-A79BACD4C03B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D60D4E91-FAF8-FA45-ACFF-F80C010D1587}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6340" yWindow="620" windowWidth="35040" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="3360" yWindow="620" windowWidth="35040" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -354,7 +354,7 @@
   </si>
   <si>
     <t xml:space="preserve">- Angrist and Pischke (MM), Chapter 3 (pp 98-146)
-- Come prepared to discuss backwards design of your group project. </t>
+- Come prepared to discuss `backwards design of your group project. &lt;https://github.com/nickeubank/unifyingdatascience/blob/master/project/20_BackwardsDesign/UDS_BackwardsDesign_Assignment.pdf&gt;`_ </t>
   </si>
 </sst>
 </file>
@@ -761,7 +761,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -988,7 +988,7 @@
       <c r="C17" s="11"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" ht="51">
+    <row r="18" spans="1:4" ht="102">
       <c r="A18" s="2" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
update for covid19 schedule
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA06B83A-5B4D-0E4C-A8C0-6578E4498C24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EDBCD1D-990C-664E-9E4B-64766B595A98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="620" windowWidth="35040" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="2400" yWindow="460" windowWidth="35040" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="84">
   <si>
     <t>Topic</t>
   </si>
@@ -353,6 +353,15 @@
 - `Diversity in AI is not your problem, it's hers &lt;https://medium.com/@robert.munro/bias-in-ai-3ea569f79d6a&gt;`_
 - `Not all AI bias is unintentional... &lt;https://www.washingtonpost.com/nation/2020/01/28/opioid-kickback-software/&gt;`_
 - `Again, not all unintentional... &lt;https://www.vice.com/en_us/article/epgmbw/this-company-is-using-racially-biased-algorithms-to-select-jurors&gt;`_</t>
+  </si>
+  <si>
+    <t>SPRING RECESS, COVID-19 EDITION</t>
+  </si>
+  <si>
+    <t>- **Revised Project Proposal Due**</t>
+  </si>
+  <si>
+    <t>??</t>
   </si>
 </sst>
 </file>
@@ -758,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1014,47 +1023,57 @@
       </c>
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="1:4" ht="119">
+    <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="372">
+      <c r="B21" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="B22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="119">
       <c r="A23" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="B23" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>50</v>
+      </c>
       <c r="D23" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" ht="372">
       <c r="A24" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
+      <c r="B24" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="B25" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
@@ -1066,6 +1085,9 @@
       <c r="C26" s="3" t="s">
         <v>52</v>
       </c>
+      <c r="D26" s="8" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2" t="s">
@@ -1093,12 +1115,16 @@
       <c r="A29" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="1"/>
+      <c r="B29" s="3" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
         <v>45</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update class schedule readings
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EDBCD1D-990C-664E-9E4B-64766B595A98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C90EC8-FD30-5943-AEC4-7DE12A2F5E37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="460" windowWidth="35040" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="2380" yWindow="460" windowWidth="35040" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -347,21 +347,25 @@
 - Come prepared to discuss `backwards design of your group project. &lt;https://github.com/nickeubank/unifyingdatascience/blob/master/project/20_BackwardsDesign/UDS_BackwardsDesign_Assignment.pdf&gt;`_ </t>
   </si>
   <si>
-    <t>- `ProPublica: Machine Bias &lt;https://www.propublica.org/article/machine-bias-risk-assessments-in-criminal-sentencing&gt;`_
+    <t>SPRING RECESS, COVID-19 EDITION</t>
+  </si>
+  <si>
+    <t>- **Revised Project Proposal Due**</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>**Required:**
+- `ProPublica: Machine Bias &lt;https://www.propublica.org/article/machine-bias-risk-assessments-in-criminal-sentencing&gt;`_
+- `ProPublica Analysis of COMPAS &lt;https://www.propublica.org/article/how-we-analyzed-the-compas-recidivism-algorithm&gt;`_
 - `Racial Bias in Medical Algorithm &lt;https://www.washingtonpost.com/health/2019/10/24/racial-bias-medical-algorithm-favors-white-patients-over-sicker-black-patients/&gt;`_
 - `Amazon scraps secret AI recruiting tool due to bias &lt;https://www.reuters.com/article/us-amazon-com-jobs-automation-insight/amazon-scraps-secret-ai-recruiting-tool-that-showed-bias-against-women-idUSKCN1MK08G&gt;`_
+- `Not all AI bias is unintentional... &lt;https://www.washingtonpost.com/nation/2020/01/28/opioid-kickback-software/&gt;`_
+- `Openning the Black Box:` &lt;https://pratt.duke.edu/about/news/podcast/opening-black-box&gt;`_
+**Optional:**
 - `Diversity in AI is not your problem, it's hers &lt;https://medium.com/@robert.munro/bias-in-ai-3ea569f79d6a&gt;`_
-- `Not all AI bias is unintentional... &lt;https://www.washingtonpost.com/nation/2020/01/28/opioid-kickback-software/&gt;`_
 - `Again, not all unintentional... &lt;https://www.vice.com/en_us/article/epgmbw/this-company-is-using-racially-biased-algorithms-to-select-jurors&gt;`_</t>
-  </si>
-  <si>
-    <t>SPRING RECESS, COVID-19 EDITION</t>
-  </si>
-  <si>
-    <t>- **Revised Project Proposal Due**</t>
-  </si>
-  <si>
-    <t>??</t>
   </si>
 </sst>
 </file>
@@ -768,14 +772,14 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="21.83203125" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="49.33203125" customWidth="1"/>
+    <col min="3" max="3" width="80.6640625" customWidth="1"/>
     <col min="4" max="4" width="50.5" style="6" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1028,7 +1032,7 @@
         <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1036,7 +1040,7 @@
         <v>37</v>
       </c>
       <c r="B22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="119">
@@ -1053,7 +1057,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="372">
+    <row r="24" spans="1:4" ht="356">
       <c r="A24" s="2" t="s">
         <v>39</v>
       </c>
@@ -1061,7 +1065,7 @@
         <v>47</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1069,10 +1073,10 @@
         <v>40</v>
       </c>
       <c r="B25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1086,7 +1090,7 @@
         <v>52</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1116,7 +1120,7 @@
         <v>44</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1124,7 +1128,7 @@
         <v>45</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update readings and schedule
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9A49F10-142B-2043-95A6-F87569E5829F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{FB5CE8D2-9F65-CC46-B963-DFA81EF1ABFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2380" yWindow="460" windowWidth="35040" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -353,20 +353,20 @@
     <t>??</t>
   </si>
   <si>
-    <t>**Required:**
+    <t>- **Final Project Proposal Due**
+- `Slides &lt;https://github.com/nickeubank/unifyingdatascience/blob/master/lecture_slides/50_prediction/Eubank_UDS_prediction_handout.pdf&gt;`_</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> **Required:**
 - `ProPublica: Machine Bias &lt;https://www.propublica.org/article/machine-bias-risk-assessments-in-criminal-sentencing&gt;`_
 - `ProPublica Analysis of COMPAS &lt;https://www.propublica.org/article/how-we-analyzed-the-compas-recidivism-algorithm&gt;`_
 - `Racial Bias in Medical Algorithm &lt;https://www.washingtonpost.com/health/2019/10/24/racial-bias-medical-algorithm-favors-white-patients-over-sicker-black-patients/&gt;`_
 - `Amazon scraps secret AI recruiting tool due to bias &lt;https://www.reuters.com/article/us-amazon-com-jobs-automation-insight/amazon-scraps-secret-ai-recruiting-tool-that-showed-bias-against-women-idUSKCN1MK08G&gt;`_
 - `Not all AI bias is unintentional... &lt;https://www.washingtonpost.com/nation/2020/01/28/opioid-kickback-software/&gt;`_
-- `Openning the Black Box:` &lt;https://pratt.duke.edu/about/news/podcast/opening-black-box&gt;`_
+- `Openning the Black Box: &lt;https://pratt.duke.edu/about/news/podcast/opening-black-box&gt;`_
 **Optional:**
 - `Diversity in AI is not your problem, it's hers &lt;https://medium.com/@robert.munro/bias-in-ai-3ea569f79d6a&gt;`_
 - `Again, not all unintentional... &lt;https://www.vice.com/en_us/article/epgmbw/this-company-is-using-racially-biased-algorithms-to-select-jurors&gt;`_</t>
-  </si>
-  <si>
-    <t>- **Final Project Proposal Due**
-- `Slides &lt;https://github.com/nickeubank/unifyingdatascience/blob/master/lecture_slides/50_prediction/Eubank_UDS_prediction_handout.pdf&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -773,7 +773,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1055,10 +1055,10 @@
         <v>49</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="356">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="340">
       <c r="A24" s="2" t="s">
         <v>39</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>47</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:4">

</xml_diff>

<commit_message>
add cheatsheet to site
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6080EA-AB6C-A44E-9535-702EA067FF9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C439093-F352-E840-A596-B6B51E429DA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2380" yWindow="460" windowWidth="35040" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="87">
   <si>
     <t>Topic</t>
   </si>
@@ -350,9 +350,6 @@
     <t>- **Revised Project Proposal Due**</t>
   </si>
   <si>
-    <t>??</t>
-  </si>
-  <si>
     <t>- **Final Project Proposal Due**
 - `Slides &lt;https://github.com/nickeubank/unifyingdatascience/blob/master/lecture_slides/50_prediction/Eubank_UDS_prediction_handout.pdf&gt;`_</t>
   </si>
@@ -373,6 +370,12 @@
   </si>
   <si>
     <t>Modelling of Presentations and Feedback</t>
+  </si>
+  <si>
+    <t>Course Summary Class</t>
+  </si>
+  <si>
+    <t>- `Summary Cheatsheet &lt;https://github.com/nickeubank/unifyingdatascience/blob/master/lecture_slides/80_final_cheatsheet/UDS_Final_Cheatsheet.pdf&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -779,7 +782,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1061,7 +1064,7 @@
         <v>49</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="340">
@@ -1072,7 +1075,7 @@
         <v>47</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1080,10 +1083,10 @@
         <v>40</v>
       </c>
       <c r="B25" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" t="s">
         <v>84</v>
-      </c>
-      <c r="C25" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1127,15 +1130,21 @@
         <v>44</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
+        <v>50</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="68">
       <c r="A30" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>81</v>
+        <v>85</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update first presentation and schedule
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D23F5F-31DF-AD48-AA8B-4CAC52F2CBD9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774625E3-7F96-1949-BAA2-657AAB062E9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3360" yWindow="500" windowWidth="35040" windowHeight="19480" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="87">
   <si>
     <t>Topic</t>
   </si>
@@ -292,32 +292,6 @@
   </si>
   <si>
     <t>Tues, Apr 20</t>
-  </si>
-  <si>
-    <t>**NO CLASS*</t>
-  </si>
-  <si>
-    <r>
-      <t>- Angrist and Piscke (MHE) Part 1 (p</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="SFBX1200"/>
-      </rPr>
-      <t>ages 3-24)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="SFRM1200"/>
-      </rPr>
-      <t xml:space="preserve">
-- Review linear regression in Python (`WM Chapter &lt;https://www.amazon.com/Python-Data-Analysis-Wrangling-IPython-ebook/dp/B075X4LT6K&gt;`_ 13, 13.1, 13.2, 13.3)
-- `Experiments in Advertising &lt;https://overcast.fm/+QLduPjO1I&gt;`_</t>
-    </r>
   </si>
   <si>
     <t>- Internal v. External Validity
@@ -377,6 +351,39 @@
   <si>
     <t>- `Taxonomy of Questions &lt;taxonomy_of_questions.ipynb&gt;`_
 - **Backwards Design Due**</t>
+  </si>
+  <si>
+    <t>**NO CLASS**</t>
+  </si>
+  <si>
+    <t>Wellness Day</t>
+  </si>
+  <si>
+    <t>Thurs, Apr 22</t>
+  </si>
+  <si>
+    <r>
+      <t>- Angrist and Piscke (MHE) Part 1 (p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="SFBX1200"/>
+      </rPr>
+      <t>ages 3-24)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="SFRM1200"/>
+      </rPr>
+      <t xml:space="preserve">
+- Review linear regression in Python (`WM Chapter &lt;https://www.amazon.com/Python-Data-Analysis-Wrangling-IPython-ebook/dp/B075X4LT6K&gt;`_ 13, 13.1, 13.2, 13.3)
+- Asymptotics and Linear Probability Models
+- `Experiments in Advertising &lt;https://overcast.fm/+QLduPjO1I&gt;`_</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -783,10 +790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -820,7 +827,7 @@
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="68">
@@ -831,7 +838,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>28</v>
@@ -851,7 +858,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="68">
+    <row r="5" spans="1:4" ht="85">
       <c r="A5" s="2" t="s">
         <v>51</v>
       </c>
@@ -859,7 +866,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>30</v>
@@ -870,10 +877,10 @@
         <v>52</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>75</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>77</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>31</v>
@@ -951,13 +958,13 @@
     </row>
     <row r="12" spans="1:4" ht="72" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="68">
@@ -987,10 +994,10 @@
         <v>60</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -998,10 +1005,10 @@
         <v>61</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="29">
@@ -1012,7 +1019,7 @@
         <v>4</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>20</v>
@@ -1026,7 +1033,7 @@
         <v>6</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>21</v>
@@ -1054,7 +1061,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>46</v>
@@ -1110,10 +1117,10 @@
         <v>70</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>18</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1127,14 +1134,25 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="68">
+    <row r="27" spans="1:4">
       <c r="A27" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="68">
+      <c r="A28" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D28" s="7" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update schedule with sutva
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A344AF7C-9AFE-C84B-A79B-4A14879FAFD7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C449ECFA-B53A-DE41-8F75-20DD5AB357C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="500" windowWidth="35040" windowHeight="19480" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="2460" yWindow="500" windowWidth="35040" windowHeight="19480" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -326,11 +326,6 @@
     <t>- Freedman (SMaCI), Chapter 3</t>
   </si>
   <si>
-    <t>- `Internal versus External Validity
-- `Limitations of Average Treatment Effects &lt;limitations_of_ATE.ipynb&gt;`_
-- `Experiments in Advertising &lt;https://overcast.fm/+QLduPjO1I&gt;`_</t>
-  </si>
-  <si>
     <t>- `Interpreting Indicator Vars &lt;interpreting_indicator_vars.ipynb&gt;`_
 - Kennedy (GtE), Chpt 18.
 - `Fixed Effects v. Hierarchical Models &lt;fixed_effects_v_hierarchical.ipynb&gt;`_
@@ -353,12 +348,6 @@
       <t xml:space="preserve"> 178-208) 
 - `Backwards Design &lt;backwards_design.ipynb&gt;`_</t>
     </r>
-  </si>
-  <si>
-    <t>- Compliance / ITT / Etc.</t>
-  </si>
-  <si>
-    <t>- Angrist and Pischke (MM), Chapter 3 (pp 98-146)</t>
   </si>
   <si>
     <t>- `Potential Outcome Slides &lt;https://github.com/nickeubank/unifyingdatascience/blob/master/lecture_slides/20_PotentialOutcomes/Eubank_UDS_PotentialOutcomes_handout.pdf&gt;`_
@@ -394,6 +383,20 @@
     <t>- `Potential Outcomes &lt;https://github.com/nickeubank/unifyingdatascience/blob/master/lecture_slides/20_PotentialOutcomes/Fresh_Potential_Outcomes.pdf&gt;`_
 Optional (Alternative presentation, slightly different notation):
 - Imbens and Rubin (CI), Chpt 1.</t>
+  </si>
+  <si>
+    <t>- Internal versus External Validity
+- `Limitations of Average Treatment Effects &lt;limitations_of_ATE.ipynb&gt;`_
+- `Experiments in Advertising &lt;https://overcast.fm/+QLduPjO1I&gt;`_</t>
+  </si>
+  <si>
+    <t>- SUTVA
+- Compliance / ITT / Etc.</t>
+  </si>
+  <si>
+    <t>- Imbens and Rubin (CI), Section 1.6 (SUTVA, p. 10-13)
+- Angrist and Pischke (MM), Chapter 3 (pp 98-146)
+(Note that Imben &amp; Rubin potential outcomes notation is a little different -- just skip notational parts if needed)</t>
   </si>
 </sst>
 </file>
@@ -799,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -848,7 +851,7 @@
         <v>76</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="102">
@@ -859,7 +862,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>23</v>
@@ -873,7 +876,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>26</v>
@@ -887,21 +890,21 @@
         <v>66</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17">
+    <row r="7" spans="1:4" ht="85">
       <c r="A7" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>82</v>
+      <c r="B7" s="6" t="s">
+        <v>85</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="34">
@@ -940,7 +943,7 @@
         <v>25</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>30</v>
@@ -965,10 +968,10 @@
         <v>69</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>80</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>81</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
add endogenous stopping warning
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C449ECFA-B53A-DE41-8F75-20DD5AB357C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B76A86A-564B-7942-A104-BD6C505D9349}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="500" windowWidth="35040" windowHeight="19480" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="9880" yWindow="500" windowWidth="27620" windowHeight="19480" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -385,11 +385,6 @@
 - Imbens and Rubin (CI), Chpt 1.</t>
   </si>
   <si>
-    <t>- Internal versus External Validity
-- `Limitations of Average Treatment Effects &lt;limitations_of_ATE.ipynb&gt;`_
-- `Experiments in Advertising &lt;https://overcast.fm/+QLduPjO1I&gt;`_</t>
-  </si>
-  <si>
     <t>- SUTVA
 - Compliance / ITT / Etc.</t>
   </si>
@@ -397,6 +392,12 @@
     <t>- Imbens and Rubin (CI), Section 1.6 (SUTVA, p. 10-13)
 - Angrist and Pischke (MM), Chapter 3 (pp 98-146)
 (Note that Imben &amp; Rubin potential outcomes notation is a little different -- just skip notational parts if needed)</t>
+  </si>
+  <si>
+    <t>- Internal versus External Validity
+- `Limitations of Average Treatment Effects &lt;limitations_of_ATE.ipynb&gt;`_
+- `Endogenous Stopping Times in Experiments &lt;http://sl8r000.github.io/ab_testing_statistics/avoid_biased_stopping_times/&gt;`_
+- Optional: `Discussion in part About Experiments in Advertising &lt;https://overcast.fm/+QLduPjO1I&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -802,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -882,7 +883,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="51">
+    <row r="6" spans="1:4" ht="102">
       <c r="A6" s="2" t="s">
         <v>45</v>
       </c>
@@ -890,7 +891,7 @@
         <v>66</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>27</v>
@@ -901,10 +902,10 @@
         <v>46</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>85</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="34">

</xml_diff>

<commit_message>
add draft of internal v. external
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B76A86A-564B-7942-A104-BD6C505D9349}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3946C3B5-114F-D047-BAB5-BC6E63608E6F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9880" yWindow="500" windowWidth="27620" windowHeight="19480" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -75,9 +75,6 @@
     <t>CI: Natural Experiments</t>
   </si>
   <si>
-    <t xml:space="preserve">`Matching Methods for Causal Inference: A Review and a Look Forward &lt;https://www.ncbi.nlm.nih.gov/pmc/articles/PMC2943670/&gt;`_ </t>
-  </si>
-  <si>
     <t>Prediction: ML Bias</t>
   </si>
   <si>
@@ -140,10 +137,6 @@
   <si>
     <t>- `Indicators &lt;exercises/exercise_indicators.ipynb&gt;`_
 - `Fixed Effects &lt;exercises/exercise_panel.ipynb&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Slides &lt;https://github.com/nickeubank/unifyingdatascience/blob/master/lecture_slides/30_matching/matching.pdf&gt;`_
-- `Exercises &lt;exercises/exercise_matching.ipynb&gt;`_</t>
   </si>
   <si>
     <t>- `Link &lt;exercises/exercise_diffindiff.ipynb&gt;`_</t>
@@ -394,9 +387,17 @@
 (Note that Imben &amp; Rubin potential outcomes notation is a little different -- just skip notational parts if needed)</t>
   </si>
   <si>
-    <t>- Internal versus External Validity
+    <t>- `Exercises &lt;exercises/exercise_matching.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Matching Methods for Causal Inference: A Review and a Look Forward &lt;https://www.ncbi.nlm.nih.gov/pmc/articles/PMC2943670/&gt;`_
+- `DAME-FLAME User Guide &lt;https://almost-matching-exactly.github.io/DAME-FLAME-Python-Package/user-guide&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Internal versus External Validity &lt;internal_v_external_validity.ipynb&gt;`_
 - `Limitations of Average Treatment Effects &lt;limitations_of_ATE.ipynb&gt;`_
-- `Endogenous Stopping Times in Experiments &lt;http://sl8r000.github.io/ab_testing_statistics/avoid_biased_stopping_times/&gt;`_
+- `A/B Testing and Stopping Early &lt;https://medium.com/airbnb-engineering/experiments-at-airbnb-e2db3abf39e7&gt;`_
+- Optional: `More on endogenous stopping &lt;http://sl8r000.github.io/ab_testing_statistics/avoid_biased_stopping_times/&gt;`_
 - Optional: `Discussion in part About Experiments in Advertising &lt;https://overcast.fm/+QLduPjO1I&gt;`_</t>
   </si>
 </sst>
@@ -462,7 +463,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -477,9 +478,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -803,7 +801,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -831,340 +829,340 @@
     </row>
     <row r="2" spans="1:4" ht="113">
       <c r="A2" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="102">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>76</v>
+      <c r="C3" s="8" t="s">
+        <v>74</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="102">
       <c r="A4" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>83</v>
+      <c r="C4" s="8" t="s">
+        <v>81</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="136">
       <c r="A5" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>82</v>
+      <c r="C5" s="8" t="s">
+        <v>80</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="102">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="136">
       <c r="A6" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>86</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="85">
       <c r="A7" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="34">
       <c r="A8" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="34">
       <c r="A9" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>24</v>
+      <c r="C9" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="68">
       <c r="A10" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="68">
       <c r="A11" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>31</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="72" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>80</v>
+        <v>77</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="68">
       <c r="A13" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>33</v>
+      <c r="C13" s="8" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17">
       <c r="A14" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="29">
       <c r="A17" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="68">
       <c r="A18" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="11" t="s">
-        <v>70</v>
+      <c r="C18" s="10" t="s">
+        <v>68</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="29">
       <c r="A19" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="85">
       <c r="A20" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="404">
       <c r="A21" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="34">
       <c r="A22" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="D23" s="7"/>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="68">
       <c r="A28" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
prelim FEs and causal inference
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC34DEDB-1222-D04A-950A-F6CA28E064FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE8C600-20A3-234E-8FCC-F354B4538557}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5080" yWindow="500" windowWidth="27620" windowHeight="19480" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -412,6 +412,7 @@
   <si>
     <t>- `Interpreting Indicator Vars &lt;interpreting_indicator_vars.ipynb&gt;`_
 - `Fixed Effects v. Hierarchical Models &lt;fixed_effects_v_hierarchical.ipynb&gt;`_
+- `Fixed Effects and Causal Inference &lt;fixed_effects_and_causal_inference.ipynb&gt;`_
 - `Implementing Fixed Effects &lt;fixed_effects.ipynb&gt;`_
 Optional: 
 - Kennedy (GtE), Chpt 18.</t>
@@ -818,7 +819,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -953,7 +954,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="102">
+    <row r="10" spans="1:4" ht="119">
       <c r="A10" s="2" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
most ml doesn't make money
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC44BB56-EE68-3547-8DE6-6115F65DF827}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7AB3D0-2353-2D49-A02C-457DA9993679}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5080" yWindow="500" windowWidth="27620" windowHeight="19480" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -249,11 +249,6 @@
     <t xml:space="preserve">Thurs, Feb 25  </t>
   </si>
   <si>
-    <t xml:space="preserve">- `Moving from Problems to Questions &lt;moving_from_problems_to_questions&gt;`_
-- `Why It's Important To Get Your Question Right &lt;https://www.youtube.com/watch?v=kYMfE9u-lMo&gt;`_
-</t>
-  </si>
-  <si>
     <t>- `Taxonomy of Questions &lt;taxonomy_of_questions.ipynb&gt;`_
 - **Backwards Design Due**</t>
   </si>
@@ -418,6 +413,12 @@
 - `The How of Matching Summary &lt;matching_how.ipynb&gt;`_
 - `Methods for Matching &lt;https://youtu.be/tvMyjDi4dyg?t=910&gt;`_
 *Watch the video above from about 15 minutes in (where link starts) till at least 45 minutes in, keep going if you want to learn about propensity score matching problems.*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- `Moving from Problems to Questions &lt;moving_from_problems_to_questions&gt;`_
+- `Why It's Important To Get Your Question Right &lt;https://www.youtube.com/watch?v=kYMfE9u-lMo&gt;`_
+- `Most ML Doesn't Make Money &lt;https://www.wired.com/story/companies-rushing-use-ai-few-see-payoff/&gt;`_
+</t>
   </si>
 </sst>
 </file>
@@ -820,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -855,7 +856,7 @@
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="102">
@@ -866,10 +867,10 @@
         <v>8</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="102">
@@ -880,7 +881,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>22</v>
@@ -894,7 +895,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>24</v>
@@ -908,7 +909,7 @@
         <v>61</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>25</v>
@@ -919,13 +920,13 @@
         <v>41</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C7" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="102">
@@ -936,10 +937,10 @@
         <v>17</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="34">
@@ -950,7 +951,7 @@
         <v>11</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>26</v>
@@ -964,7 +965,7 @@
         <v>23</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>27</v>
@@ -978,10 +979,10 @@
         <v>10</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="72" customHeight="1">
@@ -989,10 +990,10 @@
         <v>64</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>72</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>73</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>28</v>
@@ -1006,7 +1007,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17">
@@ -1025,7 +1026,7 @@
         <v>48</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15" t="s">
         <v>62</v>
@@ -1036,7 +1037,7 @@
         <v>49</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C16" t="s">
         <v>62</v>
@@ -1050,13 +1051,13 @@
         <v>4</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="68">
+    <row r="18" spans="1:4" ht="102">
       <c r="A18" s="2" t="s">
         <v>51</v>
       </c>
@@ -1064,7 +1065,7 @@
         <v>6</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>19</v>
@@ -1148,10 +1149,10 @@
         <v>58</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1178,7 +1179,7 @@
     </row>
     <row r="28" spans="1:4" ht="68">
       <c r="A28" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
add Netflix endogenous stopping
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96A7F7F-1BA4-1B4C-A61C-585523AD85B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504BF56C-1740-C143-8B15-F05C86CF3315}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5080" yWindow="500" windowWidth="27620" windowHeight="19480" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -329,13 +329,6 @@
     <t>- `Exercises &lt;exercises/exercise_matching.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>- `Internal versus External Validity &lt;internal_v_external_validity.ipynb&gt;`_
-- `Limitations of Average Treatment Effects &lt;limitations_of_ATE.ipynb&gt;`_
-- `A/B Testing and Stopping Early &lt;https://medium.com/airbnb-engineering/experiments-at-airbnb-e2db3abf39e7&gt;`_
-- Optional: `More on endogenous stopping &lt;http://sl8r000.github.io/ab_testing_statistics/avoid_biased_stopping_times/&gt;`_
-- Optional: `Discussion in part About Experiments in Advertising &lt;https://overcast.fm/+QLduPjO1I&gt;`_</t>
-  </si>
-  <si>
     <t>- Freedman (SMaCI), Chapter 3
 - Imbens and Rubin (CI), Section 1.6 (SUTVA, p. 10-13)
 - `Power Calculations &lt;https://emj.bmj.com/content/emermed/20/5/453.full.pdf&gt;`_
@@ -427,6 +420,14 @@
   <si>
     <t>- CI: A/B Testing in Industry
 - Backwards Design</t>
+  </si>
+  <si>
+    <t>- `Internal versus External Validity &lt;internal_v_external_validity.ipynb&gt;`_
+- `Limitations of Average Treatment Effects &lt;limitations_of_ATE.ipynb&gt;`_
+- `A/B Testing and Stopping Early &lt;https://medium.com/airbnb-engineering/experiments-at-airbnb-e2db3abf39e7&gt;`_
+- `On Correctly Stopping A/B Tests Early &lt;https://netflixtechblog.com/improving-experimentation-efficiency-at-netflix-with-meta-analysis-and-optimal-stopping-d8ec290ae5be&gt;`_
+- Optional: `More on bad endogenous stopping &lt;http://sl8r000.github.io/ab_testing_statistics/avoid_biased_stopping_times/&gt;`_
+- Optional: `Discussion in part About Experiments in Advertising &lt;https://overcast.fm/+QLduPjO1I&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -829,8 +830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -917,7 +918,7 @@
         <v>60</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>24</v>
@@ -931,10 +932,10 @@
         <v>73</v>
       </c>
       <c r="C7" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>77</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="102">
@@ -945,10 +946,10 @@
         <v>16</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="34">
@@ -959,7 +960,7 @@
         <v>11</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>25</v>
@@ -973,7 +974,7 @@
         <v>22</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>26</v>
@@ -987,7 +988,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>74</v>
@@ -998,10 +999,10 @@
         <v>63</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>27</v>
@@ -1012,10 +1013,10 @@
         <v>45</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17">
@@ -1073,7 +1074,7 @@
         <v>6</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
fix backwards design due date
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF131032-0A37-9041-B735-CBAD4A4E1BA8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5AFFA3A-478B-7E4B-AC27-43AD48E08F19}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5080" yWindow="500" windowWidth="27620" windowHeight="19480" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -246,10 +246,6 @@
     <t xml:space="preserve">Thurs, Feb 25  </t>
   </si>
   <si>
-    <t>- `Taxonomy of Questions &lt;taxonomy_of_questions.ipynb&gt;`_
-- **Backwards Design Due**</t>
-  </si>
-  <si>
     <t>**NO CLASS**</t>
   </si>
   <si>
@@ -435,9 +431,13 @@
 - Two Stage Least Squares</t>
   </si>
   <si>
+    <t>- `Taxonomy of Questions &lt;taxonomy_of_questions.ipynb&gt;`_</t>
+  </si>
+  <si>
     <t>- Angrist and Pischke (MM), Chapter 3, Sections 3.3 - End
-- Angrist and Pischke (MM), Chapter 4
-- `RDD at Coursera &lt;https://medium.com/coursera-engineering/regression-discontinuity-understanding-the-benefit-of-subtitles-on-coursera-dd82bb25a0f1&gt;`_</t>
+- Morgan and Winship, Chapter 11
+- `RDD at Coursera &lt;https://medium.com/coursera-engineering/regression-discontinuity-understanding-the-benefit-of-subtitles-on-coursera-dd82bb25a0f1&gt;`_
+- **Backwards Design Due**</t>
   </si>
 </sst>
 </file>
@@ -874,7 +874,7 @@
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="102">
@@ -885,10 +885,10 @@
         <v>8</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>69</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="102">
@@ -899,7 +899,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>21</v>
@@ -913,7 +913,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>23</v>
@@ -927,7 +927,7 @@
         <v>60</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>24</v>
@@ -938,13 +938,13 @@
         <v>40</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C7" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="102">
@@ -955,10 +955,10 @@
         <v>16</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="68">
@@ -969,7 +969,7 @@
         <v>11</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>25</v>
@@ -983,7 +983,7 @@
         <v>22</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>26</v>
@@ -997,10 +997,10 @@
         <v>10</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="72" customHeight="1">
@@ -1008,10 +1008,10 @@
         <v>63</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>27</v>
@@ -1022,10 +1022,10 @@
         <v>45</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17">
@@ -1044,7 +1044,7 @@
         <v>47</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s">
         <v>61</v>
@@ -1055,18 +1055,18 @@
         <v>48</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C16" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="68">
+    <row r="17" spans="1:4" ht="85">
       <c r="A17" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>89</v>
@@ -1080,7 +1080,7 @@
         <v>4</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>17</v>
@@ -1094,7 +1094,7 @@
         <v>6</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>18</v>
@@ -1166,10 +1166,10 @@
         <v>57</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1196,7 +1196,7 @@
     </row>
     <row r="28" spans="1:4" ht="68">
       <c r="A28" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
update schedule and syllabus
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{53606857-4EB4-FC4E-80FE-C3570EE3943E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915550C6-CA78-2244-BFAA-F76CC8DE1E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="2200" windowWidth="39220" windowHeight="19160" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="680" yWindow="1780" windowWidth="30400" windowHeight="19080" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="95">
   <si>
     <t>Topic</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>7 minute presentations + 7 minutes of questions per group</t>
-  </si>
-  <si>
-    <t>CI: Ghost Map</t>
   </si>
   <si>
     <t>`Types of Questions &lt;exercises/exercise_taxonomy_of_questions.ipynb&gt;`_</t>
@@ -137,30 +134,6 @@
   <si>
     <t>- `Welcome! Slides Part 1 &lt;https://github.com/nickeubank/unifyingdatascience/blob/master/lecture_slides/10_FirstClass/Eubank_UDS_FirstClass_Part1_handout.pdf&gt;`_
 - `Welcome! Slides Part 2 &lt;https://github.com/nickeubank/unifyingdatascience/blob/master/lecture_slides/10_FirstClass/Eubank_UDS_FirstClass_Part2_handout.pdf&gt;`_</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">- Read Angrist and Piscke (MM), </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="SFBX1200"/>
-      </rPr>
-      <t>Pages xi - 30</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="SFRM1200"/>
-      </rPr>
-      <t xml:space="preserve">
-- Read, sign, submit syllabus on gradescope. 
-- `Submit substantive interest survey &lt;https://forms.gle/cpr9SB4d7unXRx3j6&gt;`_
-- Submit Reading Reflections on Gradescope.</t>
-    </r>
   </si>
   <si>
     <t>- `Potential Outcome Slides &lt;https://github.com/nickeubank/unifyingdatascience/blob/master/lecture_slides/20_PotentialOutcomes/Eubank_UDS_PotentialOutcomes_handout.pdf&gt;`_
@@ -193,20 +166,11 @@
     </r>
   </si>
   <si>
-    <t>- `Potential Outcomes &lt;https://github.com/nickeubank/unifyingdatascience/blob/master/lecture_slides/20_PotentialOutcomes/Fresh_Potential_Outcomes.pdf&gt;`_
-Optional (Alternative presentation, slightly different notation):
-- Imbens and Rubin (CI), Chpt 1.</t>
-  </si>
-  <si>
     <t>- `Exercises &lt;exercises/exercise_matching.ipynb&gt;`_</t>
   </si>
   <si>
     <t>- `Evaluating Studies &lt;exercises/exercise_evaluating_studies.ipynb&gt;`_
 - `Redo HW &lt;exercises/exercise_potential_outcomes2.ipynb&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Link 1 &lt;exercises/exercise_ghostmap_1.ipynb&gt;`_
-- `Link 2 &lt;exercises/exercise_ghostmap_2.ipynb&gt;`_</t>
   </si>
   <si>
     <t>- `Interpreting Indicator Vars &lt;interpreting_indicator_vars.ipynb&gt;`_
@@ -227,10 +191,6 @@
 - `Why It's Important To Get Your Question Right &lt;https://www.youtube.com/watch?v=kYMfE9u-lMo&gt;`_
 - `Most ML Doesn't Make Money &lt;https://www.wired.com/story/companies-rushing-use-ai-few-see-payoff/&gt;`_
 </t>
-  </si>
-  <si>
-    <t>- Kohavi, Tang and Xu, Chapters 2, 5, 22
-- `Backwards Design &lt;backwards_design.ipynb&gt;`_</t>
   </si>
   <si>
     <r>
@@ -258,10 +218,6 @@
     <t>- CI: Difference-in-Differences</t>
   </si>
   <si>
-    <t>- CI: A/B Testing in Industry
-- Backwards Design</t>
-  </si>
-  <si>
     <t>- `Internal versus External Validity &lt;internal_v_external_validity.ipynb&gt;`_
 - `Limitations of Average Treatment Effects &lt;limitations_of_ATE.ipynb&gt;`_
 - `A/B Testing and Stopping Early &lt;https://medium.com/airbnb-engineering/experiments-at-airbnb-e2db3abf39e7&gt;`_
@@ -418,16 +374,6 @@
   </si>
   <si>
     <t>CI: AB Testing / Experiments</t>
-  </si>
-  <si>
-    <t>CI: AB Testing / Experiments
-- SUTVA
-- Compliance / ITT / Etc.</t>
-  </si>
-  <si>
-    <t>CI: AB Testing / Experiments
-- Experiments with Spillovers (Networks)
-- Power Calculations</t>
   </si>
   <si>
     <r>
@@ -453,24 +399,76 @@
     </r>
   </si>
   <si>
-    <t>- Freedman (SMaCI), Chapter 3
-- `Power Calculations &lt;https://emj.bmj.com/content/emermed/20/5/453.full.pdf&gt;`_
-- `Bias in A/B Testing &lt;https://medium.com/airbnb-engineering/selection-bias-in-online-experimentation-c3d67795cceb&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Evaluating Studies &lt;evaluating_real_studies.ipynb&gt;`_
-- Angrist and Pischke (MM), Chapter 3 (pp 98-123)
-- Imbens and Rubin (CI), Section 1.6 (SUTVA, p. 10-13)
-(Note that Imben &amp; Rubin potential outcomes notation is a little different -- just skip notational parts if needed)</t>
-  </si>
-  <si>
-    <t>`- Thinking about AB Testing Discussion
-- Link &lt;exercises/exercise_abtesting.ipynb&gt;`_</t>
+    <r>
+      <t xml:space="preserve">- Read, sign, submit syllabus on gradescope. 
+- `Submit substantive interest survey &lt;https://forms.gle/cpr9SB4d7unXRx3j6&gt;`_
+- Read Angrist and Piscke (MM), </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="SFBX1200"/>
+      </rPr>
+      <t>Pages xi - 30
+- `Potential Outcomes &lt;https://github.com/nickeubank/unifyingdatascience/blob/master/lecture_slides/20_PotentialOutcomes/Fresh_Potential_Outcomes.pdf&gt;`_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="SFRM1200"/>
+      </rPr>
+      <t xml:space="preserve">
+- Submit Reading Reflections on Gradescope.</t>
+    </r>
+  </si>
+  <si>
+    <t>`- Link &lt;exercises/exercise_abtesting.ipynb&gt;`_
+- Thinking about AB Testing Discussion</t>
   </si>
   <si>
     <t>CI: AB Testing / Experiments
 - Limitations of Experiments and ATE
-- Internal v. External Validity</t>
+- Internal v. External Validity
+- Stopping Early</t>
+  </si>
+  <si>
+    <t>- Kohavi, Tang and Xu, Chpts 5, 19
+- Angrist and Pischke (MM), Chapter 3 (pp 98-123)</t>
+  </si>
+  <si>
+    <t>- `Evaluating Studies &lt;evaluating_real_studies.ipynb&gt;`_
+- Imbens and Rubin (CI), Section 1.6 (SUTVA, p. 10-13)
+- Kohavi, Tang and Xu, Intro - Chpt 4, 22
+(Note that Imben &amp; Rubin potential outcomes notation is a little different -- just skip notational parts if needed)</t>
+  </si>
+  <si>
+    <t>CI: AB Testing / Experiments
+- Evaluating studies
+- Testing in industry
+- SUTVA</t>
+  </si>
+  <si>
+    <t>- `Bias in A/B Testing &lt;https://medium.com/airbnb-engineering/selection-bias-in-online-experimentation-c3d67795cceb&gt;`_
+- Kohavi, Tang and Xu, Chpt 3
+- `Power Calculations &lt;https://emj.bmj.com/content/emermed/20/5/453.full.pdf&gt;`_</t>
+  </si>
+  <si>
+    <t>Experiments recap</t>
+  </si>
+  <si>
+    <t>CI: AB Testing / Experiments
+- Compliance</t>
+  </si>
+  <si>
+    <t>- Backwards Design</t>
+  </si>
+  <si>
+    <t>- `Backwards Design &lt;backwards_design.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>Questions?</t>
   </si>
 </sst>
 </file>
@@ -875,8 +873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -903,324 +901,328 @@
     </row>
     <row r="2" spans="1:4" ht="113">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="102">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="119">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>33</v>
+        <v>83</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="102">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>36</v>
-      </c>
+      <c r="C4" s="6"/>
       <c r="D4" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="136">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="247" customHeight="1">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="102">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>88</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="85">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="51">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="68">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="34">
-      <c r="A9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
       <c r="D9" s="5" t="s">
-        <v>39</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="51">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="167" customHeight="1">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="72" customHeight="1">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="51">
       <c r="A13" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="68">
+      <c r="A14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="34">
-      <c r="A14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="68">
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>51</v>
+        <v>65</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="103" customHeight="1">
       <c r="A17" t="s">
-        <v>73</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>50</v>
+        <v>67</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>52</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="63" customHeight="1">
       <c r="A18" t="s">
-        <v>74</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>49</v>
+        <v>68</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="136">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="29">
       <c r="A21" t="s">
-        <v>77</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>71</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="68">
       <c r="A22" t="s">
-        <v>78</v>
+        <v>72</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="29">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="409.6">
       <c r="A24" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="255">
       <c r="A25" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="102">
       <c r="A26" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="34">
       <c r="A27" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>13</v>
@@ -1231,18 +1233,18 @@
     </row>
     <row r="29" spans="1:4" ht="68">
       <c r="A29" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="B30" s="2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add reading reflection directions
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915550C6-CA78-2244-BFAA-F76CC8DE1E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF0CEEC-845D-C24D-AD05-7339D297DD44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="1780" windowWidth="30400" windowHeight="19080" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="680" yWindow="1040" windowWidth="30400" windowHeight="19080" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="96">
   <si>
     <t>Topic</t>
   </si>
@@ -399,9 +399,56 @@
     </r>
   </si>
   <si>
+    <t>`- Link &lt;exercises/exercise_abtesting.ipynb&gt;`_
+- Thinking about AB Testing Discussion</t>
+  </si>
+  <si>
+    <t>CI: AB Testing / Experiments
+- Limitations of Experiments and ATE
+- Internal v. External Validity
+- Stopping Early</t>
+  </si>
+  <si>
+    <t>- Kohavi, Tang and Xu, Chpts 5, 19
+- Angrist and Pischke (MM), Chapter 3 (pp 98-123)</t>
+  </si>
+  <si>
+    <t>- `Evaluating Studies &lt;evaluating_real_studies.ipynb&gt;`_
+- Imbens and Rubin (CI), Section 1.6 (SUTVA, p. 10-13)
+- Kohavi, Tang and Xu, Intro - Chpt 4, 22
+(Note that Imben &amp; Rubin potential outcomes notation is a little different -- just skip notational parts if needed)</t>
+  </si>
+  <si>
+    <t>CI: AB Testing / Experiments
+- Evaluating studies
+- Testing in industry
+- SUTVA</t>
+  </si>
+  <si>
+    <t>- `Bias in A/B Testing &lt;https://medium.com/airbnb-engineering/selection-bias-in-online-experimentation-c3d67795cceb&gt;`_
+- Kohavi, Tang and Xu, Chpt 3
+- `Power Calculations &lt;https://emj.bmj.com/content/emermed/20/5/453.full.pdf&gt;`_</t>
+  </si>
+  <si>
+    <t>Experiments recap</t>
+  </si>
+  <si>
+    <t>CI: AB Testing / Experiments
+- Compliance</t>
+  </si>
+  <si>
+    <t>- Backwards Design</t>
+  </si>
+  <si>
+    <t>- `Backwards Design &lt;backwards_design.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>Questions?</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">- Read, sign, submit syllabus on gradescope. 
-- `Submit substantive interest survey &lt;https://forms.gle/cpr9SB4d7unXRx3j6&gt;`_
+      <t xml:space="preserve">- Read, sign, submit syllabus on gradescope.
+- Reading Reflections Directions &lt;reading_reflectips.ipynb&gt;`_
 - Read Angrist and Piscke (MM), </t>
     </r>
     <r>
@@ -424,51 +471,8 @@
     </r>
   </si>
   <si>
-    <t>`- Link &lt;exercises/exercise_abtesting.ipynb&gt;`_
-- Thinking about AB Testing Discussion</t>
-  </si>
-  <si>
-    <t>CI: AB Testing / Experiments
-- Limitations of Experiments and ATE
-- Internal v. External Validity
-- Stopping Early</t>
-  </si>
-  <si>
-    <t>- Kohavi, Tang and Xu, Chpts 5, 19
-- Angrist and Pischke (MM), Chapter 3 (pp 98-123)</t>
-  </si>
-  <si>
-    <t>- `Evaluating Studies &lt;evaluating_real_studies.ipynb&gt;`_
-- Imbens and Rubin (CI), Section 1.6 (SUTVA, p. 10-13)
-- Kohavi, Tang and Xu, Intro - Chpt 4, 22
-(Note that Imben &amp; Rubin potential outcomes notation is a little different -- just skip notational parts if needed)</t>
-  </si>
-  <si>
-    <t>CI: AB Testing / Experiments
-- Evaluating studies
-- Testing in industry
-- SUTVA</t>
-  </si>
-  <si>
-    <t>- `Bias in A/B Testing &lt;https://medium.com/airbnb-engineering/selection-bias-in-online-experimentation-c3d67795cceb&gt;`_
-- Kohavi, Tang and Xu, Chpt 3
-- `Power Calculations &lt;https://emj.bmj.com/content/emermed/20/5/453.full.pdf&gt;`_</t>
-  </si>
-  <si>
-    <t>Experiments recap</t>
-  </si>
-  <si>
-    <t>CI: AB Testing / Experiments
-- Compliance</t>
-  </si>
-  <si>
-    <t>- Backwards Design</t>
-  </si>
-  <si>
-    <t>- `Backwards Design &lt;backwards_design.ipynb&gt;`_</t>
-  </si>
-  <si>
-    <t>Questions?</t>
+    <t>- `Submit substantive interest survey &lt;https://forms.gle/cpr9SB4d7unXRx3j6&gt;`_
+- No reading reflections due.</t>
   </si>
 </sst>
 </file>
@@ -873,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -919,20 +923,22 @@
         <v>8</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17">
+    <row r="4" spans="1:4" ht="34">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="6" t="s">
+        <v>95</v>
+      </c>
       <c r="D4" s="5" t="s">
         <v>18</v>
       </c>
@@ -948,7 +954,7 @@
         <v>33</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="247" customHeight="1">
@@ -956,7 +962,7 @@
         <v>56</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>41</v>
@@ -970,10 +976,10 @@
         <v>57</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>35</v>
@@ -984,10 +990,10 @@
         <v>58</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="68">
@@ -998,10 +1004,10 @@
         <v>81</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="51">
@@ -1076,7 +1082,7 @@
         <v>65</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17">
@@ -1095,10 +1101,10 @@
         <v>67</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>92</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="63" customHeight="1">

</xml_diff>

<commit_message>
Add reading on P values
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F96513-A603-AA4C-94BE-9A4B1F821D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF380E3-113A-7F4C-B3B1-BC2D3FFEB56D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="500" windowWidth="30300" windowHeight="19180" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="3040" yWindow="10500" windowWidth="30300" windowHeight="19180" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -441,8 +441,19 @@
 (Note that Imben &amp; Rubin potential outcomes notation is a little different -- just skip notational parts if needed)</t>
   </si>
   <si>
+    <t>- `Bias in A/B Testing &lt;https://medium.com/airbnb-engineering/selection-bias-in-online-experimentation-c3d67795cceb&gt;`_
+- `Bias in Research &lt;https://www.youtube.com/watch?v=42QuXLucH3Q&gt;`_
+- `Power Calculations &lt;https://cxl.com/blog/statistical-power/&gt;`_
+- Kohavi, Tang, and Xu, Chpt 23
+- Angrist and Pischke (MM), Chapter 3 (pp 98-123)</t>
+  </si>
+  <si>
+    <t>- Kohavi, Tang and Xu, Chpts 1, 2, 3, 5, 19, 22</t>
+  </si>
+  <si>
     <r>
-      <t>- `Causal Inference In Industry Beyond AB Testing &lt;causal_inference_beyond_ab_testing.ipynb`_
+      <t>- `Causal Inference In Industry Beyond AB Testing &lt;causal_inference_beyond_ab_testing.ipynb&gt;`_
+- `Moving to a World Beyond p less than 0.05 &lt;https://www.tandfonline.com/doi/full/10.1080/00031305.2019.1583913&gt; `_
 - Angrist and Piscke (MM), Chapter 2 (pp. 47-82)</t>
     </r>
     <r>
@@ -453,16 +464,6 @@
       </rPr>
       <t xml:space="preserve">. </t>
     </r>
-  </si>
-  <si>
-    <t>- `Bias in A/B Testing &lt;https://medium.com/airbnb-engineering/selection-bias-in-online-experimentation-c3d67795cceb&gt;`_
-- `Bias in Research &lt;https://www.youtube.com/watch?v=42QuXLucH3Q&gt;`_
-- `Power Calculations &lt;https://cxl.com/blog/statistical-power/&gt;`_
-- Kohavi, Tang, and Xu, Chpt 23
-- Angrist and Pischke (MM), Chapter 3 (pp 98-123)</t>
-  </si>
-  <si>
-    <t>- Kohavi, Tang and Xu, Chpts 1, 2, 3, 5, 19, 22</t>
   </si>
 </sst>
 </file>
@@ -867,7 +868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -983,7 +984,7 @@
         <v>43</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17">
@@ -994,7 +995,7 @@
         <v>43</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="245" customHeight="1">
@@ -1005,7 +1006,7 @@
         <v>47</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>46</v>
@@ -1019,7 +1020,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>80</v>

</xml_diff>

<commit_message>
update potential outcome solutions
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3D69BAF-42EF-114E-9933-AE7768B9D5C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E930820-6DB6-6349-B515-F296DA9CD9CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3040" yWindow="2320" windowWidth="30300" windowHeight="19180" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14360" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -199,22 +199,6 @@
     - `Robograders &lt;https://www.vice.com/en_us/article/pa7dj9/flawed-algorithms-are-grading-millions-of-students-essays&gt;`_</t>
   </si>
   <si>
-    <t xml:space="preserve"> **Examples of AI Bias:**
-- `Making Biased Algorithms &lt;https://youtube.com/watch?v=Ok5sKLXqynQ&gt;`_
-- `ProPublica: Machine Bias &lt;https://www.propublica.org/article/machine-bias-risk-assessments-in-criminal-sentencing&gt;`_
-- `The Problem with Controlling for Race &lt;https://www.nejm.org/doi/10.1056/NEJMms2004740&gt;`_
-- `Racial Bias in Medical Algorithm &lt;https://www.washingtonpost.com/health/2019/10/24/racial-bias-medical-algorithm-favors-white-patients-over-sicker-black-patients/&gt;`_
-- `Amazon scraps secret AI recruiting tool due to bias &lt;https://www.reuters.com/article/us-amazon-com-jobs-automation-insight/amazon-scraps-secret-ai-recruiting-tool-that-showed-bias-against-women-idUSKCN1MK08G&gt;`_
-- `Algorithm Blocks Kidney Transplants to Black Patients &lt;https://www.wired.com/story/how-algorithm-blocked-kidney-transplants-black-patients/&gt;`_
-- `Algorithms and Student Exams &lt;https://www.theguardian.com/education/2021/feb/18/the-student-and-the-algorithm-how-the-exam-results-fiasco-threatened-one-pupils-future&gt;`_
-- `Not all AI bias is unintentional... &lt;https://www.washingtonpost.com/nation/2020/01/28/opioid-kickback-software/&gt;`_
-- `Again, not all unintentional... &lt;https://www.vice.com/en_us/article/epgmbw/this-company-is-using-racially-biased-algorithms-to-select-jurors&gt;`_
-**Optional:**
-- `ProPublica Analysis of COMPAS &lt;https://www.propublica.org/article/how-we-analyzed-the-compas-recidivism-algorithm&gt;`_
-- `Diversity in AI is not your problem, it's hers &lt;https://medium.com/@robert.munro/bias-in-ai-3ea569f79d6a&gt;`_
-**GITHUB REPO FIRST REVIEW**</t>
-  </si>
-  <si>
     <t xml:space="preserve">- `Recommendations for Ethical ML &lt;ethical_ml_recommendations.ipynb&gt;`_
 - `In Defence of Simplicity (Up to 30min) &lt;https://www.youtube.com/watch?v=68ABAU_V8qI&gt;`_
 - `Stop Using Black Boxes &lt;https://arxiv.org/abs/1811.10154&gt;`_
@@ -454,6 +438,23 @@
     <t>- Angrist and Piscke (MM), Chapter 2 (pp. 47-82). 
 - `Causal Inference In Industry Beyond AB Testing &lt;causal_inference_beyond_ab_testing.ipynb&gt;`_
 - `Moving to a World Beyond p less than 0.05 &lt;https://www.tandfonline.com/doi/full/10.1080/00031305.2019.1583913&gt;`_</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> **Examples of AI Bias:**
+- `Making Biased Algorithms &lt;https://youtube.com/watch?v=Ok5sKLXqynQ&gt;`_
+- `ProPublica: Machine Bias &lt;https://www.propublica.org/article/machine-bias-risk-assessments-in-criminal-sentencing&gt;`_
+- `The Problem with Controlling for Race &lt;https://www.nejm.org/doi/10.1056/NEJMms2004740&gt;`_
+- `Racial Bias in Medical Algorithm &lt;https://www.washingtonpost.com/health/2019/10/24/racial-bias-medical-algorithm-favors-white-patients-over-sicker-black-patients/&gt;`_
+- `Amazon scraps secret AI recruiting tool due to bias &lt;https://www.reuters.com/article/us-amazon-com-jobs-automation-insight/amazon-scraps-secret-ai-recruiting-tool-that-showed-bias-against-women-idUSKCN1MK08G&gt;`_
+- `Algorithm Blocks Kidney Transplants to Black Patients &lt;https://www.wired.com/story/how-algorithm-blocked-kidney-transplants-black-patients/&gt;`_
+- `Algorithms and Student Exams &lt;https://www.theguardian.com/education/2021/feb/18/the-student-and-the-algorithm-how-the-exam-results-fiasco-threatened-one-pupils-future&gt;`_
+- `Algorithms in Hiring &lt;https://www.youtube.com/watch?v=6nGM37ThEsU&gt;`_
+- `Not all AI bias is unintentional... &lt;https://www.washingtonpost.com/nation/2020/01/28/opioid-kickback-software/&gt;`_
+- `Again, not all unintentional... &lt;https://www.vice.com/en_us/article/epgmbw/this-company-is-using-racially-biased-algorithms-to-select-jurors&gt;`_
+**Optional:**
+- `ProPublica Analysis of COMPAS &lt;https://www.propublica.org/article/how-we-analyzed-the-compas-recidivism-algorithm&gt;`_
+- `Diversity in AI is not your problem, it's hers &lt;https://medium.com/@robert.munro/bias-in-ai-3ea569f79d6a&gt;`_
+**GITHUB REPO FIRST REVIEW**</t>
   </si>
 </sst>
 </file>
@@ -858,8 +859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -886,7 +887,7 @@
     </row>
     <row r="2" spans="1:4" ht="113">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>7</v>
@@ -898,13 +899,13 @@
     </row>
     <row r="3" spans="1:4" ht="119">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>29</v>
@@ -912,119 +913,119 @@
     </row>
     <row r="4" spans="1:4" ht="34">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="136">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>30</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="247" customHeight="1">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>33</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="102">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="245" customHeight="1">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="167" customHeight="1">
       <c r="A11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="72" customHeight="1">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>19</v>
@@ -1032,7 +1033,7 @@
     </row>
     <row r="13" spans="1:4" ht="119">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>9</v>
@@ -1041,18 +1042,18 @@
         <v>31</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="119">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>20</v>
@@ -1060,10 +1061,10 @@
     </row>
     <row r="15" spans="1:4" ht="68">
       <c r="A15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>35</v>
@@ -1071,7 +1072,7 @@
     </row>
     <row r="16" spans="1:4" ht="17">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>24</v>
@@ -1082,18 +1083,18 @@
     </row>
     <row r="17" spans="1:4" ht="103" customHeight="1">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="63" customHeight="1">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>6</v>
@@ -1104,7 +1105,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>27</v>
@@ -1115,7 +1116,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>27</v>
@@ -1126,7 +1127,7 @@
     </row>
     <row r="21" spans="1:4" ht="29">
       <c r="A21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>4</v>
@@ -1140,10 +1141,10 @@
     </row>
     <row r="22" spans="1:4" ht="68">
       <c r="A22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>36</v>
@@ -1151,7 +1152,7 @@
     </row>
     <row r="23" spans="1:4" ht="29">
       <c r="A23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>5</v>
@@ -1165,29 +1166,29 @@
     </row>
     <row r="24" spans="1:4" ht="409.6">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>39</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="255">
       <c r="A25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>37</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="102">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>12</v>
@@ -1196,12 +1197,12 @@
         <v>38</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="34">
       <c r="A27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B27" t="s">
         <v>21</v>
@@ -1212,7 +1213,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>13</v>
@@ -1223,7 +1224,7 @@
     </row>
     <row r="29" spans="1:4" ht="68">
       <c r="A29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>22</v>
@@ -1234,7 +1235,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="B30" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add good notebook reading
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37496697-988C-5B4E-B595-D221C43C8AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C50D44-C64F-D745-AB7A-CA7D952308A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3160" yWindow="500" windowWidth="35240" windowHeight="19420" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17460" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -373,7 +373,8 @@
 - `Passive Prediction &lt;https://ds4humans.com/30_questions/20_passive_prediction_questions.html&gt;`_</t>
   </si>
   <si>
-    <t>- Read Angrist and Piscke (MM), Pages xi - 30
+    <t>- `Writing Good Notebooks &lt;https://www.practicaldatascience.org/html/writing_good_jupyter_notebooks.html&gt;`_
+- Read Angrist and Piscke (MM), Pages xi - 30
 - `Potential Outcomes &lt;https://github.com/nickeubank/unifyingdatascience/blob/master/lecture_slides/20_PotentialOutcomes/Fresh_Potential_Outcomes.pdf&gt;`_</t>
   </si>
 </sst>
@@ -791,7 +792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -882,7 +883,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="69" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="86" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
update schedule and readings
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE822315-5BF1-B342-BA93-8923F9A261D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{CF80A72D-06D5-564B-A9B3-5F1F008A214E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17460" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="94">
   <si>
     <t>Topic</t>
   </si>
@@ -283,10 +283,6 @@
 - `Limitations of Average Treatment Effects &lt;limitations_of_ATE.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>What is AB Testing? KTX Chpts 1, 2, 5
-[DO I WANT DISCUSSION OF PRACTICAL V STATISTICAL HERE?]</t>
-  </si>
-  <si>
     <t>- `Internal versus External Validity &lt;internal_v_external_validity.ipynb&gt;`_
 - `Evaluating Studies &lt;evaluating_real_studies.ipynb&gt;`_</t>
   </si>
@@ -316,14 +312,6 @@
     <t>Diff-in-Diff</t>
   </si>
   <si>
-    <t>- `What makes good teams? &lt;https://www.youtube.com/watch?v=LhoLuui9gX8&gt;`_
-- Project Aristotle Reading
-- Do teamwork prep sent on Sakai.</t>
-  </si>
-  <si>
-    <t>AB: Overview</t>
-  </si>
-  <si>
     <t>AB: Internal Validity</t>
   </si>
   <si>
@@ -347,9 +335,6 @@
     <t>Backwards Design</t>
   </si>
   <si>
-    <t>Teams</t>
-  </si>
-  <si>
     <t>Stakeholder Management</t>
   </si>
   <si>
@@ -378,14 +363,56 @@
 - `Potential Outcomes &lt;https://github.com/nickeubank/unifyingdatascience/blob/master/lecture_slides/20_PotentialOutcomes/Fresh_Potential_Outcomes.pdf&gt;`_</t>
   </si>
   <si>
-    <t>Team Debriefs</t>
+    <t>Teams 1</t>
+  </si>
+  <si>
+    <t>- Exercise &lt;exercises/exercise_counterfactuals.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <r>
+      <t>- Angrist and Piscke (MHE) Part 1 (p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="SFBX1200"/>
+      </rPr>
+      <t>ages 3-24)
+- Kennedy (GtE), pp. 18-21, Notes for 2.8
+- Kennedy (GtE), pp. 241-244, Notes Optional</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="SFRM1200"/>
+      </rPr>
+      <t xml:space="preserve">
+- Review linear regression in Python (`WM Chapter &lt;https://www.amazon.com/Python-Data-Analysis-Wrangling-IPython-ebook/dp/B075X4LT6K&gt;`_ 13, 13.1, 13.2, 13.3) 
+Optional:
+- Wooldridge, Section 15.2</t>
+    </r>
+  </si>
+  <si>
+    <t>AB: Regression Implementations</t>
+  </si>
+  <si>
+    <t>Teams 2</t>
+  </si>
+  <si>
+    <t>- `What makes good teams? &lt;https://www.youtube.com/watch?v=LhoLuui9gX8&gt;`_
+- `Project Aristotle Reading &lt;https://github.com/nickeubank/unifyingdatascience/raw/master/team_readings/project_aristotle_nytimes.pdf&gt;`_</t>
+  </si>
+  <si>
+    <t>- Do teamwork prep sent on Sakai.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -426,6 +453,16 @@
       <color rgb="FF000000"/>
       <name val="Fira Code"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="SFRM1200"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="SFBX1200"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -447,7 +484,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -477,6 +514,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -795,11 +835,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="17.5" customWidth="1"/>
     <col min="2" max="2" width="31" style="2" customWidth="1"/>
@@ -807,7 +847,7 @@
     <col min="4" max="4" width="50.5" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -821,7 +861,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="121" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="121">
       <c r="A2" s="10" t="s">
         <v>30</v>
       </c>
@@ -833,7 +873,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="69" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="69">
       <c r="A3" s="10" t="s">
         <v>31</v>
       </c>
@@ -841,27 +881,27 @@
         <v>59</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="35" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="35">
       <c r="A4" s="10" t="s">
         <v>32</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="119" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="119" customHeight="1">
       <c r="A5" s="10" t="s">
         <v>33</v>
       </c>
@@ -869,10 +909,10 @@
         <v>60</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="247" customHeight="1" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="247" customHeight="1">
       <c r="A6" s="10" t="s">
         <v>34</v>
       </c>
@@ -880,13 +920,13 @@
         <v>61</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="86" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="86">
       <c r="A7" s="10" t="s">
         <v>35</v>
       </c>
@@ -894,147 +934,150 @@
         <v>62</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="137">
       <c r="A8" s="10" t="s">
         <v>36</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="72" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="52">
       <c r="A9" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="245" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="245" customHeight="1">
       <c r="A10" s="10" t="s">
         <v>38</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="167" customHeight="1" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="167" customHeight="1">
       <c r="A11" s="10" t="s">
         <v>39</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>66</v>
+        <v>73</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="72" customHeight="1">
       <c r="A12" s="10" t="s">
         <v>40</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="58" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30">
       <c r="A13" s="10" t="s">
         <v>41</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="52" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="58">
       <c r="A14" s="10" t="s">
         <v>42</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="D14" s="8"/>
-    </row>
-    <row r="15" spans="1:4" ht="35" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="52">
       <c r="A15" s="10" t="s">
         <v>43</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="144" customHeight="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:4" ht="144" customHeight="1">
       <c r="A16" s="10" t="s">
         <v>44</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C16" t="s">
-        <v>81</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="103" customHeight="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="103" customHeight="1">
       <c r="A17" s="10" t="s">
         <v>45</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="C17" t="s">
+        <v>78</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="63" customHeight="1">
       <c r="A18" s="10" t="s">
         <v>46</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="18">
       <c r="A19" s="10" t="s">
         <v>47</v>
       </c>
@@ -1042,7 +1085,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="18">
       <c r="A20" s="10" t="s">
         <v>48</v>
       </c>
@@ -1050,7 +1093,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="18">
       <c r="A21" s="10" t="s">
         <v>49</v>
       </c>
@@ -1058,35 +1101,33 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="103" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="188">
       <c r="A22" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>83</v>
-      </c>
+      <c r="B22" s="7"/>
       <c r="C22" s="7" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="188" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="103">
       <c r="A23" s="10" t="s">
         <v>51</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="52" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="188">
       <c r="A24" s="10" t="s">
         <v>52</v>
       </c>
@@ -1094,11 +1135,13 @@
         <v>4</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="D24" s="8"/>
-    </row>
-    <row r="25" spans="1:4" ht="154" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="154">
       <c r="A25" s="10" t="s">
         <v>53</v>
       </c>
@@ -1112,7 +1155,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="409.6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="409.6">
       <c r="A26" s="10" t="s">
         <v>54</v>
       </c>
@@ -1123,7 +1166,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="273" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="273">
       <c r="A27" s="10" t="s">
         <v>55</v>
       </c>
@@ -1132,7 +1175,7 @@
       </c>
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="1:4" ht="103" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="103">
       <c r="A28" s="10" t="s">
         <v>56</v>
       </c>
@@ -1144,7 +1187,7 @@
       </c>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:4" ht="35" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="35">
       <c r="A29" s="10" t="s">
         <v>57</v>
       </c>

</xml_diff>

<commit_message>
fix assignment for tues
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D5A33D1D-02AB-EF40-8203-667AFBA5A8F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{384C7AC5-C7B3-AF49-8181-5E4A1093B54C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4080" yWindow="500" windowWidth="30240" windowHeight="17340" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -398,9 +398,6 @@
     <t>Teams 2</t>
   </si>
   <si>
-    <t>- `Exercise &lt;exercises/exercise_counterfactuals.ipynb&gt;`_</t>
-  </si>
-  <si>
     <t>- `What Project Aristotle Learned &lt;https://github.com/nickeubank/unifyingdatascience/raw/master/team_readings/project_aristotle_nytimes.pdf&gt;`_
 - Edmondson, The Fearless Organization, Chpt 1 (on Sakai)
 Optional: `Fostering Psychological Safety &lt;https://docs.google.com/document/d/1PsnDMS2emcPLgMLFAQCXZjO7C4j2hJ7znOq_g2Zkjgk/export?format=pdf&gt;`_</t>
@@ -408,6 +405,9 @@
   <si>
     <t>- `Review Team Charter Assignment &lt;https://github.com/nickeubank/unifyingdatascience/raw/master/team_readings/MIDS%20Team%20Charter%20Assignment.docx&gt;`_
 - Edmondson, Teaming, Chpt 2 (on Sakai)</t>
+  </si>
+  <si>
+    <t>- `Exercise &lt;exercises/exercise_potential_outcomes1.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -837,7 +837,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -939,7 +939,7 @@
         <v>86</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="137">
@@ -964,7 +964,7 @@
         <v>87</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="245" customHeight="1">
@@ -975,7 +975,7 @@
         <v>90</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="167" customHeight="1">

</xml_diff>

<commit_message>
schedule formatting; git push
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65C09F3-BCC2-5044-9BBF-21201D3B19C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0C9E2854-A595-F84F-9402-A485FD46901A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1760" yWindow="520" windowWidth="33240" windowHeight="19460" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -310,6 +310,79 @@
     <t>Analyzing Experiments</t>
   </si>
   <si>
+    <t>AB: Threats to Internal Validity</t>
+  </si>
+  <si>
+    <t>Online AB Testing</t>
+  </si>
+  <si>
+    <t>AB: Analyzing A/B Tests</t>
+  </si>
+  <si>
+    <t>AB: Evaluating External Validity</t>
+  </si>
+  <si>
+    <t>AB: Making Decisions</t>
+  </si>
+  <si>
+    <t>- Seasonality Effects
+- Kohvani, Tang and Xu, Chpt 23 (Primacy Effects / Long Term Decay)
+- Representativeness</t>
+  </si>
+  <si>
+    <t>AB: Designing Experiments</t>
+  </si>
+  <si>
+    <t>- `Causal Inference In Industry Beyond AB Testing &lt;causal_inference_beyond_ab_testing.ipynb&gt;`_
+- Angrist and Piscke (MM), Chpt 2</t>
+  </si>
+  <si>
+    <t>Causality and Regression</t>
+  </si>
+  <si>
+    <t>- `Contraining Artificial Stupidity &lt;https://www.youtube.com/watch?v=Z8MEFI7ZJlA&gt;`_
+- Adversarial Users:
+    - `Fooling OpenAI &lt;https://www.theverge.com/2021/3/8/22319173/openai-machine-vision-adversarial-typographic-attacka-clip-multimodal-neuron&gt;`_
+    - `Robograders &lt;https://www.vice.com/en_us/article/pa7dj9/flawed-algorithms-are-grading-millions-of-students-essays&gt;`_
+- **PROJECT ROUGH DRAFTS DUE**</t>
+  </si>
+  <si>
+    <t>- Kohavi, Tang and Xu, Chpt 1, 2, 5 (Online AB Testing Intro)</t>
+  </si>
+  <si>
+    <t>- `Interpreting Indicator Vars &lt;interpreting_indicator_vars.ipynb&gt;`_
+- `Fixed Effects v. Hierarchical Models &lt;fixed_effects_v_hierarchical.ipynb&gt;`_
+- `Fixed Effects and Causal Inference &lt;fixed_effects_and_causal_inference.ipynb&gt;`_
+- `Implementing Fixed Effects &lt;fixed_effects.ipynb&gt;`_
+Optional: 
+- Kennedy (GtE), Chpt 18.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Kohvani, Tang and Xu Chpt 7
+- `Power Calculations &lt;https://www.povertyactionlab.org/resource/power-calculations&gt;`_
+</t>
+  </si>
+  <si>
+    <t>- P-Values and Decision Making
+- `Moving to a World Beyond p less than 0.05 &lt;https://www.tandfonline.com/doi/full/10.1080/00031305.2019.1583913&gt;`_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUTVA in AB Testing:
+- Kohavi, Tang and Xu: Chpt 3, "Threats to Internal Validity" (p. 42-47)
+- Different Randomizations: KTX Chpt 22
+Validating Internal Validity:
+- Kohvani, Tang and Xu: Chpt 19 (A/A Testing)
+- Kohvani, Tang and Xu: Chpt 21 (Guardrail Metrics)
+</t>
+  </si>
+  <si>
+    <t>Dangers of Early Stopping:
+- `Don’t stop experiments early! &lt;endogenous_stopping.ipynb&gt;`_
+-`...unless you use these methods &lt;https://netflixtechblog.com/improving-experimentation-efficiency-at-netflix-with-meta-analysis-and-optimal-stopping-d8ec290ae5be&gt;`_
+Power and Decisions:
+- Kohavi, Tang and Xu, Chpt 3 up to "Threats to Internal Validity" (p. 39-42)</t>
+  </si>
+  <si>
     <r>
       <t>Causal Theory:
 - `Limitations of Average Treatment Effects &lt;limitations_of_ATE.ipynb&gt;`_
@@ -334,79 +407,6 @@
       </rPr>
       <t>- Review linear regression in Python (`WM Chapter &lt;https://www.amazon.com/Python-Data-Analysis-Wrangling-IPython-ebook/dp/B075X4LT6K&gt;`_ 13, 13.1, 13.2, 13.3)</t>
     </r>
-  </si>
-  <si>
-    <t>AB: Threats to Internal Validity</t>
-  </si>
-  <si>
-    <t>Online AB Testing</t>
-  </si>
-  <si>
-    <t>AB: Analyzing A/B Tests</t>
-  </si>
-  <si>
-    <t>AB: Evaluating External Validity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SUTVA in AB Testing:
-- Kohavi, Tang and Xu: Chpt 3, "Threats to Internal Validity" (p. 42-47)
-- Different Randomizations: KTX Chpt 22
-Validating Internal Validity:
-- Kohvani, Tang and Xu: Chpt 19 (A/A Testing)
-- Kohvani, Tang and Xu: Chpt 21 (Guardrail Metrics)
-</t>
-  </si>
-  <si>
-    <t>AB: Making Decisions</t>
-  </si>
-  <si>
-    <t>Dangers of Early Stopping:
-- `Don’t stop experiments early! &lt;endogenous_stopping.ipynb&gt;`_
--`...unless you use these methods &lt;https://netflixtechblog.com/improving-experimentation-efficiency-at-netflix-with-meta-analysis-and-optimal-stopping-d8ec290ae5be&gt;`_
-Power and Decisions:
-- Kohavi, Tang and Xu, Chpt 3 up to "Threats to Internal Validity" (p. 39-42)</t>
-  </si>
-  <si>
-    <t>- Seasonality Effects
-- Kohvani, Tang and Xu, Chpt 23 (Primacy Effects / Long Term Decay)
-- Representativeness</t>
-  </si>
-  <si>
-    <t>AB: Designing Experiments</t>
-  </si>
-  <si>
-    <t>- `Causal Inference In Industry Beyond AB Testing &lt;causal_inference_beyond_ab_testing.ipynb&gt;`_
-- Angrist and Piscke (MM), Chpt 2</t>
-  </si>
-  <si>
-    <t>Causality and Regression</t>
-  </si>
-  <si>
-    <t>- `Contraining Artificial Stupidity &lt;https://www.youtube.com/watch?v=Z8MEFI7ZJlA&gt;`_
-- Adversarial Users:
-    - `Fooling OpenAI &lt;https://www.theverge.com/2021/3/8/22319173/openai-machine-vision-adversarial-typographic-attacka-clip-multimodal-neuron&gt;`_
-    - `Robograders &lt;https://www.vice.com/en_us/article/pa7dj9/flawed-algorithms-are-grading-millions-of-students-essays&gt;`_
-- **PROJECT ROUGH DRAFTS DUE**</t>
-  </si>
-  <si>
-    <t>- Kohavi, Tang and Xu, Chpt 1, 2, 5 (Online AB Testing Intro)</t>
-  </si>
-  <si>
-    <t>- `Interpreting Indicator Vars &lt;interpreting_indicator_vars.ipynb&gt;`_
-- `Fixed Effects v. Hierarchical Models &lt;fixed_effects_v_hierarchical.ipynb&gt;`_
-- `Fixed Effects and Causal Inference &lt;fixed_effects_and_causal_inference.ipynb&gt;`_
-- `Implementing Fixed Effects &lt;fixed_effects.ipynb&gt;`_
-Optional: 
-- Kennedy (GtE), Chpt 18.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Kohvani, Tang and Xu Chpt 7
-- `Power Calculations &lt;https://www.povertyactionlab.org/resource/power-calculations&gt;`_
-</t>
-  </si>
-  <si>
-    <t>- P-Values and Decision Making
-- `Moving to a World Beyond p less than 0.05 &lt;https://www.tandfonline.com/doi/full/10.1080/00031305.2019.1583913&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -837,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -986,7 +986,7 @@
         <v>74</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>53</v>
@@ -997,24 +997,24 @@
         <v>31</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="120">
+    <row r="13" spans="1:4" ht="154">
       <c r="A13" s="10" t="s">
         <v>32</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="35">
@@ -1022,21 +1022,21 @@
         <v>33</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="114">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="142">
       <c r="A15" s="10" t="s">
         <v>34</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="52">
@@ -1044,10 +1044,10 @@
         <v>35</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="44">
@@ -1055,10 +1055,10 @@
         <v>36</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="18">
@@ -1104,10 +1104,10 @@
         <v>41</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>13</v>
@@ -1118,10 +1118,10 @@
         <v>42</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>89</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>5</v>
@@ -1192,7 +1192,7 @@
       </c>
       <c r="B29" s="9"/>
       <c r="C29" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
flip ab to after general
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{82E59C88-E561-F94D-BC9C-8BCDF6A29171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5456BABA-71D0-BB48-8A6E-6F8BEFBBB3D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1760" yWindow="520" windowWidth="33240" windowHeight="19460" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="280" yWindow="500" windowWidth="33240" windowHeight="19460" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="87">
   <si>
     <t>Topic</t>
   </si>
@@ -72,9 +72,6 @@
 - `The How of Matching Summary &lt;matching_how.ipynb&gt;`_
 - `Methods for Matching &lt;https://youtu.be/tvMyjDi4dyg?t=910&gt;`_
 *Watch the video above from about 15 minutes in (where link starts) till at least 45 minutes in, keep going if you want to learn about propensity score matching problems.*</t>
-  </si>
-  <si>
-    <t>Experiments recap</t>
   </si>
   <si>
     <t>- `Backwards Design &lt;backwards_design.ipynb&gt;`_</t>
@@ -130,14 +127,6 @@
 (Don't expect to follow everything in that... just a heads up it exists!) </t>
   </si>
   <si>
-    <t>- Angrist and Piscke (MM), Chapter 5 (pp 178-208) 
-- `Diff-in-Diffs at Netflix &lt;https://netflixtechblog.com/key-challenges-with-quasi-experiments-at-netflix-89b4f234b852&gt;`_
-Optional but encouraged:
-(dont need to follow everything, 
-but here's a real diff-in-diff)
-- `Enfranchisement and Incarceration &lt;https://www.cambridge.org/core/journals/american-political-science-review/article/enfranchisement-and-incarceration-after-the-1965-voting-rights-act/C68FA7BB8CA313BDD8D9A39BA666A21D&gt;`_</t>
-  </si>
-  <si>
     <t>Thrs, Jan 12</t>
   </si>
   <si>
@@ -241,12 +230,6 @@
   </si>
   <si>
     <t>Diff-in-Diff</t>
-  </si>
-  <si>
-    <t>AB: Review</t>
-  </si>
-  <si>
-    <t>Review Exercise</t>
   </si>
   <si>
     <t>Stakeholder Management</t>
@@ -310,27 +293,9 @@
     <t>Analyzing Experiments</t>
   </si>
   <si>
-    <t>AB: Threats to Internal Validity</t>
-  </si>
-  <si>
-    <t>Online AB Testing</t>
-  </si>
-  <si>
-    <t>AB: Analyzing A/B Tests</t>
-  </si>
-  <si>
-    <t>AB: Evaluating External Validity</t>
-  </si>
-  <si>
-    <t>AB: Making Decisions</t>
-  </si>
-  <si>
     <t>- Seasonality Effects
 - Kohvani, Tang and Xu, Chpt 23 (Primacy Effects / Long Term Decay)
 - Representativeness</t>
-  </si>
-  <si>
-    <t>AB: Designing Experiments</t>
   </si>
   <si>
     <t>- `Causal Inference In Industry Beyond AB Testing &lt;causal_inference_beyond_ab_testing.ipynb&gt;`_
@@ -348,19 +313,6 @@
   </si>
   <si>
     <t>- Kohavi, Tang and Xu, Chpt 1, 2, 5 (Online AB Testing Intro)</t>
-  </si>
-  <si>
-    <t>- `Interpreting Indicator Vars &lt;interpreting_indicator_vars.ipynb&gt;`_
-- `Fixed Effects v. Hierarchical Models &lt;fixed_effects_v_hierarchical.ipynb&gt;`_
-- `Fixed Effects and Causal Inference &lt;fixed_effects_and_causal_inference.ipynb&gt;`_
-- `Implementing Fixed Effects &lt;fixed_effects.ipynb&gt;`_
-Optional: 
-- Kennedy (GtE), Chpt 18.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Kohvani, Tang and Xu Chpt 7
-- `Power Calculations &lt;https://www.povertyactionlab.org/resource/power-calculations&gt;`_
-</t>
   </si>
   <si>
     <t xml:space="preserve">SUTVA in AB Testing:
@@ -406,6 +358,36 @@
   </si>
   <si>
     <t>- Georgiev, Chpt 11</t>
+  </si>
+  <si>
+    <t>- `Interpreting Indicator Vars &lt;interpreting_indicator_vars.ipynb&gt;`_
+- `Fixed Effects v. Hierarchical Models &lt;fixed_effects_v_hierarchical.ipynb&gt;`_
+- `Fixed Effects and Causal Inference &lt;fixed_effects_and_causal_inference.ipynb&gt;`_
+- `Implementing Fixed Effects &lt;fixed_effects.ipynb&gt;`_
+Optional: 
+- Kennedy (GtE), Chpt 18.</t>
+  </si>
+  <si>
+    <t>- Angrist and Piscke (MM), Chapter 5 (pp 178-208) 
+- `Diff-in-Diffs at Netflix &lt;https://netflixtechblog.com/key-challenges-with-quasi-experiments-at-netflix-89b4f234b852&gt;`_
+Optional but encouraged:
+(dont need to follow everything, but here's a real diff-in-diff)
+- `Enfranchisement and Incarceration &lt;https://www.cambridge.org/core/journals/american-political-science-review/article/enfranchisement-and-incarceration-after-the-1965-voting-rights-act/C68FA7BB8CA313BDD8D9A39BA666A21D&gt;`_</t>
+  </si>
+  <si>
+    <t>Online AB: Overview</t>
+  </si>
+  <si>
+    <t>Online AB: Making Decisions</t>
+  </si>
+  <si>
+    <t>Online AB: Analyzing</t>
+  </si>
+  <si>
+    <t>Online AB: Internal Validity</t>
+  </si>
+  <si>
+    <t>Online AB: External Validity</t>
   </si>
 </sst>
 </file>
@@ -484,11 +466,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -836,366 +815,351 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="17.5" customWidth="1"/>
-    <col min="2" max="2" width="31" style="2" customWidth="1"/>
+    <col min="2" max="2" width="31" style="1" customWidth="1"/>
     <col min="3" max="3" width="113.33203125" customWidth="1"/>
-    <col min="4" max="4" width="50.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="50.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="121">
+      <c r="A2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="69">
+      <c r="A3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="35">
+      <c r="A4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="119" customHeight="1">
+      <c r="A5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="121">
-      <c r="A2" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="69">
-      <c r="A3" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="C5" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="247" customHeight="1">
+      <c r="A6" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C6" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="86">
+      <c r="A7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="35">
-      <c r="A4" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" s="12" t="s">
+    </row>
+    <row r="8" spans="1:4" ht="35">
+      <c r="A8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="103">
+      <c r="A9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="C9" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="76" customHeight="1">
+      <c r="A10" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="141" customHeight="1">
+      <c r="A11" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="72" customHeight="1">
+      <c r="A12" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="137">
+      <c r="A13" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="103">
+      <c r="A14" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="171">
+      <c r="A15" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="18">
+      <c r="A16" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="154">
+      <c r="A17" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="18">
+      <c r="A18" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="18">
+      <c r="A19" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="24" customHeight="1">
+      <c r="A20" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="103" customHeight="1">
+      <c r="A21" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="63" customHeight="1">
+      <c r="A22" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="52">
+      <c r="A23" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="154">
+      <c r="A24" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="409.6">
+      <c r="A25" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="273">
+      <c r="A26" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="7"/>
+    </row>
+    <row r="27" spans="1:4" ht="120">
+      <c r="A27" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="119" customHeight="1">
-      <c r="A5" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="247" customHeight="1">
-      <c r="A6" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="86">
-      <c r="A7" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="35">
-      <c r="A8" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="103">
-      <c r="A9" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="76" customHeight="1">
-      <c r="A10" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="141" customHeight="1">
-      <c r="A11" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="72" customHeight="1">
-      <c r="A12" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="154">
-      <c r="A13" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="18">
-      <c r="A14" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="142">
-      <c r="A15" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="52">
-      <c r="A16" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="44">
-      <c r="A17" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="18">
-      <c r="A18" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="18">
-      <c r="A19" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="24" customHeight="1">
-      <c r="A20" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="103" customHeight="1">
-      <c r="A21" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="63" customHeight="1">
-      <c r="A22" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="154">
-      <c r="A23" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="103">
-      <c r="A24" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="188">
-      <c r="A25" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="154">
-      <c r="A26" s="10" t="s">
+    <row r="28" spans="1:4" ht="18">
+      <c r="A28" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="409.6">
-      <c r="A27" s="10" t="s">
+      <c r="B28" s="4"/>
+    </row>
+    <row r="29" spans="1:4" ht="18">
+      <c r="A29" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="273">
-      <c r="A28" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D28" s="8"/>
-    </row>
-    <row r="29" spans="1:4" ht="120">
-      <c r="A29" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>17</v>
-      </c>
+      <c r="B29" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
fix end of schedule
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{8E38E44F-2DD3-0B42-9C9B-4DB8AD2776DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E9D30A2C-3333-6F4C-9368-783048C3E449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="500" windowWidth="33240" windowHeight="19460" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="90">
   <si>
     <t>Topic</t>
   </si>
@@ -94,39 +94,6 @@
     <t>- `Writing to Stakeholders &lt;writing_to_stakeholders.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>- `Computers v. Crime &lt;https://www.pbs.org/video/computers-v-crime-um7cco/&gt;`_
-(Hang in there past the obligatory "what is an algorithm"—it's sophisticated later)  
-**Examples of AI Bias:**
-- `Making Biased Algorithms &lt;https://youtube.com/watch?v=Ok5sKLXqynQ&gt;`_
-- `ProPublica: Machine Bias &lt;https://www.propublica.org/article/machine-bias-risk-assessments-in-criminal-sentencing&gt;`_
-- `The Problem with the Wrong Optimization Function &lt;https://www.wsj.com/articles/facebook-knows-it-encourages-division-top-executives-nixed-solutions-11590507499&gt;`_
-- `The Problem with Controlling for Race &lt;https://www.nejm.org/doi/10.1056/NEJMms2004740&gt;`_
-- `Racial Bias in Medical Algorithm &lt;https://www.washingtonpost.com/health/2019/10/24/racial-bias-medical-algorithm-favors-white-patients-over-sicker-black-patients/&gt;`_
-- `Amazon scraps secret AI recruiting tool due to bias &lt;https://www.reuters.com/article/us-amazon-com-jobs-automation-insight/amazon-scraps-secret-ai-recruiting-tool-that-showed-bias-against-women-idUSKCN1MK08G&gt;`_
-- `Algorithm Blocks Kidney Transplants to Black Patients &lt;https://www.wired.com/story/how-algorithm-blocked-kidney-transplants-black-patients/&gt;`_
-- `Algorithms and Student Exams &lt;https://www.theguardian.com/education/2021/feb/18/the-student-and-the-algorithm-how-the-exam-results-fiasco-threatened-one-pupils-future&gt;`_
-- `Algorithms in Hiring &lt;https://www.youtube.com/watch?v=6nGM37ThEsU&gt;`_
-- `Not all AI bias is unintentional... &lt;https://www.washingtonpost.com/nation/2020/01/28/opioid-kickback-software/&gt;`_
-- `Again, not all unintentional... &lt;https://www.vice.com/en_us/article/epgmbw/this-company-is-using-racially-biased-algorithms-to-select-jurors&gt;`_
-**Optional:**
-- `ProPublica Analysis of COMPAS &lt;https://www.propublica.org/article/how-we-analyzed-the-compas-recidivism-algorithm&gt;`_
-- `Diversity in AI is not your problem, it's hers &lt;https://medium.com/@robert.munro/bias-in-ai-3ea569f79d6a&gt;`_
-**GITHUB REPO FIRST REVIEW**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- `Recommendations for Ethical ML &lt;ethical_ml_recommendations.ipynb&gt;`_
-- `What IS fair? &lt;https://www.vox.com/future-perfect/22916602/ai-bias-fairness-tradeoffs-artificial-intelligence&gt;`_
-- `Black box models require trusting data too &lt;https://www.nytimes.com/2017/06/13/opinion/how-computers-are-harming-criminal-justice.html&gt;`_
-- `In Defence of Simplicity (Up to 30min) &lt;https://www.youtube.com/watch?v=68ABAU_V8qI&gt;`_
-- `Stop Using Black Boxes &lt;https://arxiv.org/abs/1811.10154&gt;`_
-- `Flavors of Training Data Bias &lt;https://arxiv.org/pdf/1901.10002.pdf&gt;`_
-**Optional:**
-- `Openning the Black Box &lt;https://pratt.duke.edu/about/news/podcast/opening-black-box&gt;`_
-- `Accuracy of Interpretable Models &lt;https://hdsr.mitpress.mit.edu/pub/f9kuryi8/release/6&gt;`_
-- `Combining explicit models and black boxes in Scientific ML &lt;https://notamonadtutorial.com/scientific-machine-learning-with-julia-the-sciml-ecosystem-b22802951c8a&gt;`_
-(Don't expect to follow everything in that... just a heads up it exists!) </t>
-  </si>
-  <si>
     <t>Thrs, Jan 12</t>
   </si>
   <si>
@@ -294,13 +261,6 @@
   </si>
   <si>
     <t>Causality and Regression</t>
-  </si>
-  <si>
-    <t>- `Contraining Artificial Stupidity &lt;https://www.youtube.com/watch?v=Z8MEFI7ZJlA&gt;`_
-- Adversarial Users:
-    - `Fooling OpenAI &lt;https://www.theverge.com/2021/3/8/22319173/openai-machine-vision-adversarial-typographic-attacka-clip-multimodal-neuron&gt;`_
-    - `Robograders &lt;https://www.vice.com/en_us/article/pa7dj9/flawed-algorithms-are-grading-millions-of-students-essays&gt;`_
-- **PROJECT ROUGH DRAFTS DUE**</t>
   </si>
   <si>
     <t>- Kohavi, Tang and Xu, Chpt 1, 2, 5 (Online AB Testing Intro)</t>
@@ -388,6 +348,38 @@
   <si>
     <t>- `Review Team Charter Assignment &lt;https://github.com/nickeubank/unifyingdatascience/raw/master/team_readings/MIDS%20Team%20Charter%20Assignment.docx&gt;`_
 Optional: `Fostering Psychological Safety Tips &lt;https://docs.google.com/document/d/1PsnDMS2emcPLgMLFAQCXZjO7C4j2hJ7znOq_g2Zkjgk/export?format=pdf&gt;`_</t>
+  </si>
+  <si>
+    <t>Algorithmic Fairness</t>
+  </si>
+  <si>
+    <t>Interpretable Models</t>
+  </si>
+  <si>
+    <t>- Mayson: ` Bias In, Bias Out &lt;https://www.yalelawjournal.org/article/bias-in-bias-out&gt;`_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- `Why are we using Black Boxes? &lt;https://hdsr.mitpress.mit.edu/pub/f9kuryi8/release/8&gt;`_
+- `Stop Using Black Boxes &lt;https://arxiv.org/abs/1811.10154&gt;`_
+- `Recommendations for Ethical ML &lt;ethical_ml_recommendations.ipynb&gt;`_
+**Optional:**
+- `Black box models require trusting data too &lt;https://www.nytimes.com/2017/06/13/opinion/how-computers-are-harming-criminal-justice.html&gt;`_
+- `Openning the Black Box &lt;https://pratt.duke.edu/about/news/podcast/opening-black-box&gt;`_
+- `Accuracy of Interpretable Models &lt;https://hdsr.mitpress.mit.edu/pub/f9kuryi8/release/6&gt;`_
+- `Combining explicit models and black boxes in Scientific ML &lt;https://notamonadtutorial.com/scientific-machine-learning-with-julia-the-sciml-ecosystem-b22802951c8a&gt;`_
+(Don't expect to follow everything in that... just a heads up it exists!) </t>
+  </si>
+  <si>
+    <t>Alignment</t>
+  </si>
+  <si>
+    <t>- `AI Safety / Misalignment &lt;https://www.youtube.com/watch?v=pYXy-A4siMw&amp;t=539s&gt;`_
+- `Alignment in ChatGPT &lt;https://youtu.be/viJt_DXTfwA&gt;`_
+- `Contraining Artificial Stupidity &lt;https://www.youtube.com/watch?v=Z8MEFI7ZJlA&gt;`_
+- Adversarial Users:
+    - `Fooling OpenAI &lt;https://www.theverge.com/2021/3/8/22319173/openai-machine-vision-adversarial-typographic-attacka-clip-multimodal-neuron&gt;`_
+    - `Robograders &lt;https://www.vice.com/en_us/article/pa7dj9/flawed-algorithms-are-grading-millions-of-students-essays&gt;`_
+- **PROJECT ROUGH DRAFTS DUE**</t>
   </si>
 </sst>
 </file>
@@ -815,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -838,12 +830,12 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="121">
       <c r="A2" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>3</v>
@@ -855,27 +847,27 @@
     </row>
     <row r="3" spans="1:4" ht="69">
       <c r="A3" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="35">
       <c r="A4" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>15</v>
@@ -883,24 +875,24 @@
     </row>
     <row r="5" spans="1:4" ht="119" customHeight="1">
       <c r="A5" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="247" customHeight="1">
       <c r="A6" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>4</v>
@@ -908,77 +900,77 @@
     </row>
     <row r="7" spans="1:4" ht="86">
       <c r="A7" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="35">
       <c r="A8" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="69">
       <c r="A9" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="76" customHeight="1">
       <c r="A10" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="141" customHeight="1">
       <c r="A11" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="72" customHeight="1">
       <c r="A12" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>12</v>
@@ -986,13 +978,13 @@
     </row>
     <row r="13" spans="1:4" ht="137">
       <c r="A13" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>5</v>
@@ -1000,10 +992,10 @@
     </row>
     <row r="14" spans="1:4" ht="103">
       <c r="A14" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>10</v>
@@ -1014,13 +1006,13 @@
     </row>
     <row r="15" spans="1:4" ht="171">
       <c r="A15" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>6</v>
@@ -1028,21 +1020,21 @@
     </row>
     <row r="16" spans="1:4" ht="18">
       <c r="A16" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="18">
       <c r="A17" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>7</v>
@@ -1050,18 +1042,18 @@
     </row>
     <row r="18" spans="1:4" ht="154">
       <c r="A18" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" s="11" t="s">
         <v>81</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="18">
       <c r="A19" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>8</v>
@@ -1069,7 +1061,7 @@
     </row>
     <row r="20" spans="1:4" ht="24" customHeight="1">
       <c r="A20" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>8</v>
@@ -1077,40 +1069,40 @@
     </row>
     <row r="21" spans="1:4" ht="103" customHeight="1">
       <c r="A21" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="63" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="18">
       <c r="A23" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="154">
       <c r="A24" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>11</v>
@@ -1119,31 +1111,38 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="409.6">
+    <row r="25" spans="1:4" ht="18">
       <c r="A25" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="239">
+      <c r="A26" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D26" s="7"/>
+    </row>
+    <row r="27" spans="1:4" ht="154">
+      <c r="A27" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="273">
-      <c r="A26" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26" s="7"/>
-    </row>
-    <row r="27" spans="1:4" ht="120">
-      <c r="A27" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27" s="4"/>
+      <c r="B27" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="C27" s="6" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>16</v>
@@ -1151,13 +1150,13 @@
     </row>
     <row r="28" spans="1:4" ht="18">
       <c r="A28" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B28" s="4"/>
     </row>
     <row r="29" spans="1:4" ht="18">
       <c r="A29" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B29" s="8"/>
     </row>

</xml_diff>

<commit_message>
mental health schedule change
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D1C82A-BA3E-9C4D-9424-1C12757F2B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD593ED-25B8-FD45-9CBD-0C6491038652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="97">
   <si>
     <t>Topic</t>
   </si>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t>- `Stakeholder Management &lt;exercises/exercise_generating_questions.ipynb&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Writing to Stakeholders &lt;writing_to_stakeholders.ipynb&gt;`_</t>
   </si>
   <si>
     <t>Thrs, Jan 12</t>
@@ -323,20 +320,6 @@
     <t>Online AB: External Validity</t>
   </si>
   <si>
-    <t xml:space="preserve">- `Why are we using Black Boxes? &lt;https://hdsr.mitpress.mit.edu/pub/f9kuryi8/release/8&gt;`_
-- `Stop Using Black Boxes &lt;https://arxiv.org/abs/1811.10154&gt;`_
-- `Recommendations for Ethical ML &lt;ethical_ml_recommendations.ipynb&gt;`_
-**Optional:**
-- `Black box models require trusting data too &lt;https://www.nytimes.com/2017/06/13/opinion/how-computers-are-harming-criminal-justice.html&gt;`_
-- `Openning the Black Box &lt;https://pratt.duke.edu/about/news/podcast/opening-black-box&gt;`_
-- `Accuracy of Interpretable Models &lt;https://hdsr.mitpress.mit.edu/pub/f9kuryi8/release/6&gt;`_
-- `Combining explicit models and black boxes in Scientific ML &lt;https://notamonadtutorial.com/scientific-machine-learning-with-julia-the-sciml-ecosystem-b22802951c8a&gt;`_
-(Don't expect to follow everything in that... just a heads up it exists!) </t>
-  </si>
-  <si>
-    <t>Alignment</t>
-  </si>
-  <si>
     <t>- `What Project Aristotle Learned &lt;https://github.com/nickeubank/unifyingdatascience/raw/master/team_readings/project_aristotle_nytimes.pdf&gt;`_
 - Edmondson, The Fearless Organization, Chpt 1 (on Sakai)</t>
   </si>
@@ -389,17 +372,35 @@
 </t>
   </si>
   <si>
-    <t>- `AI Safety / Misalignment &lt;https://www.youtube.com/watch?v=pYXy-A4siMw&amp;t=539s&gt;`_
-- `Alignment in ChatGPT &lt;https://youtu.be/viJt_DXTfwA&gt;`_
+    <t>- Kohavi, Tang and Xu, Chpt 3, "Threats to External Validity" to end (p. 47-54)
+- Kohvai, Tang and Xu, Chpt 23 (Primacy Effects / Long Term Decay)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- `AI Safety / Misalignment &lt;https://www.youtube.com/watch?v=pYXy-A4siMw&amp;t=539s&gt;`_
 - `Contraining Artificial Stupidity &lt;https://www.youtube.com/watch?v=Z8MEFI7ZJlA&gt;`_
 - Adversarial Users:
     - `Fooling OpenAI &lt;https://www.theverge.com/2021/3/8/22319173/openai-machine-vision-adversarial-typographic-attacka-clip-multimodal-neuron&gt;`_
     - `Robograders &lt;https://www.vice.com/en_us/article/pa7dj9/flawed-algorithms-are-grading-millions-of-students-essays&gt;`_
+</t>
+  </si>
+  <si>
+    <t>EXTRAS</t>
+  </si>
+  <si>
+    <t>Stuff that didn't make it to class</t>
+  </si>
+  <si>
+    <t>- `Stop Using Black Boxes &lt;https://arxiv.org/abs/1811.10154&gt;`_
+- `Writing to Stakeholders &lt;writing_to_stakeholders.ipynb&gt;`_
+**Optional:**
+- `Black box models require trusting data too &lt;https://www.nytimes.com/2017/06/13/opinion/how-computers-are-harming-criminal-justice.html&gt;`_
+- `Why are we using Black Boxes? &lt;https://hdsr.mitpress.mit.edu/pub/f9kuryi8/release/8&gt;`_
+- `Accuracy of Interpretable Models &lt;https://hdsr.mitpress.mit.edu/pub/f9kuryi8/release/6&gt;`_
+- `Combining explicit models and black boxes in Scientific ML &lt;https://notamonadtutorial.com/scientific-machine-learning-with-julia-the-sciml-ecosystem-b22802951c8a&gt;`_
 **FINAL PROJECT ROUGH DRAFTS DUE**</t>
   </si>
   <si>
-    <t>- Kohavi, Tang and Xu, Chpt 3, "Threats to External Validity" to end (p. 47-54)
-- Kohvai, Tang and Xu, Chpt 23 (Primacy Effects / Long Term Decay)</t>
+    <t>Mental Health Day</t>
   </si>
 </sst>
 </file>
@@ -832,10 +833,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -857,12 +858,12 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="121">
       <c r="A2" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>3</v>
@@ -874,27 +875,27 @@
     </row>
     <row r="3" spans="1:4" ht="69">
       <c r="A3" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="35">
       <c r="A4" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>14</v>
@@ -902,24 +903,24 @@
     </row>
     <row r="5" spans="1:4" ht="119" customHeight="1">
       <c r="A5" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="247" customHeight="1">
       <c r="A6" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>4</v>
@@ -927,77 +928,77 @@
     </row>
     <row r="7" spans="1:4" ht="86">
       <c r="A7" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="35">
       <c r="A8" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="52">
       <c r="A9" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="76" customHeight="1">
       <c r="A10" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="141" customHeight="1">
       <c r="A11" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="72" customHeight="1">
       <c r="A12" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>11</v>
@@ -1005,13 +1006,13 @@
     </row>
     <row r="13" spans="1:4" ht="137">
       <c r="A13" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>5</v>
@@ -1019,13 +1020,13 @@
     </row>
     <row r="14" spans="1:4" ht="120">
       <c r="A14" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>12</v>
@@ -1033,13 +1034,13 @@
     </row>
     <row r="15" spans="1:4" ht="171">
       <c r="A15" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>6</v>
@@ -1047,43 +1048,43 @@
     </row>
     <row r="16" spans="1:4" ht="18">
       <c r="A16" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="18">
       <c r="A17" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="18">
       <c r="A18" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="18">
       <c r="A19" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>8</v>
@@ -1091,7 +1092,7 @@
     </row>
     <row r="20" spans="1:4" ht="24" customHeight="1">
       <c r="A20" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>8</v>
@@ -1099,10 +1100,10 @@
     </row>
     <row r="21" spans="1:4" ht="178" customHeight="1">
       <c r="A21" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>10</v>
@@ -1113,7 +1114,7 @@
     </row>
     <row r="22" spans="1:4" ht="63" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>7</v>
@@ -1121,91 +1122,97 @@
     </row>
     <row r="23" spans="1:4" ht="205">
       <c r="A23" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="142">
       <c r="A24" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="35">
       <c r="A25" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="18">
       <c r="A26" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="7"/>
+    </row>
+    <row r="27" spans="1:4" ht="18">
+      <c r="A27" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="D26" s="7"/>
-    </row>
-    <row r="27" spans="1:4" ht="35">
-      <c r="A27" s="9" t="s">
+      <c r="B27" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D27" s="6"/>
+    </row>
+    <row r="28" spans="1:4" ht="18">
+      <c r="A28" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="239">
-      <c r="A28" s="9" t="s">
+      <c r="B28" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="222">
+      <c r="A29" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="171">
-      <c r="A29" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>80</v>
+      <c r="B29" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="18">
       <c r="A30" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="154">
+      <c r="A31" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>92</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add how to read and update schedule with MW reading
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF97D639-EAE4-DD48-9352-D359388AE3EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E8C7E9-A343-9D47-94F1-94356290C384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="1440" windowWidth="32780" windowHeight="19960" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="2820" yWindow="1440" windowWidth="30240" windowHeight="17300" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="98">
   <si>
     <t>Topic</t>
   </si>
@@ -85,87 +85,6 @@
     <t>- `Stakeholder Management &lt;exercises/exercise_generating_questions.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>Thrs, Jan 12</t>
-  </si>
-  <si>
-    <t>Tues, Jan 17</t>
-  </si>
-  <si>
-    <t>Thrs, Jan 19</t>
-  </si>
-  <si>
-    <t>Tues, Jan 24</t>
-  </si>
-  <si>
-    <t>Thrs, Jan 26</t>
-  </si>
-  <si>
-    <t>Tues, Jan 31</t>
-  </si>
-  <si>
-    <t>Thrs, Feb 2</t>
-  </si>
-  <si>
-    <t>Tues, Feb 7</t>
-  </si>
-  <si>
-    <t>Thrs, Feb 9</t>
-  </si>
-  <si>
-    <t>Tues, Feb 14</t>
-  </si>
-  <si>
-    <t>Thrs, Feb 16</t>
-  </si>
-  <si>
-    <t>Tues, Feb 21</t>
-  </si>
-  <si>
-    <t>Thrs, Feb 23</t>
-  </si>
-  <si>
-    <t>Tues, Feb 28</t>
-  </si>
-  <si>
-    <t>Thrs, Mar 2</t>
-  </si>
-  <si>
-    <t>Tues, Mar 7</t>
-  </si>
-  <si>
-    <t>Thrs, Mar 9</t>
-  </si>
-  <si>
-    <t>Tues, Mar 14</t>
-  </si>
-  <si>
-    <t>Thrs, Mar 16</t>
-  </si>
-  <si>
-    <t>Tues, Mar 21</t>
-  </si>
-  <si>
-    <t>Thrs, Mar 23</t>
-  </si>
-  <si>
-    <t>Tues, Mar 28</t>
-  </si>
-  <si>
-    <t>Thrs, Mar 30</t>
-  </si>
-  <si>
-    <t>Tues, Apr 4</t>
-  </si>
-  <si>
-    <t>Thrs, Apr 6</t>
-  </si>
-  <si>
-    <t>Tues, Apr 11</t>
-  </si>
-  <si>
-    <t>Thrs, Apr 13</t>
-  </si>
-  <si>
     <t>Tues, Apr 18</t>
   </si>
   <si>
@@ -207,10 +126,6 @@
   <si>
     <t>- `Descriptive versus Proscriptive Questions &lt;https://ds4humans.com/30_questions/05_descriptive_v_proscriptive.html&gt;`_
 - `Exploratory Questions &lt;https://ds4humans.com/30_questions/10_exploratory_questions.html&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Exploratory Questions (Corrected) &lt;https://ds4humans.com/30_questions/10_exploratory_questions.html&gt;`_
-- `Passive Prediction &lt;https://ds4humans.com/30_questions/20_passive_prediction_questions.html&gt;`_</t>
   </si>
   <si>
     <t>- `Writing Good Notebooks &lt;https://www.practicaldatascience.org/html/writing_good_jupyter_notebooks.html&gt;`_
@@ -348,16 +263,10 @@
     <t>Bias</t>
   </si>
   <si>
-    <t>Interpretability</t>
-  </si>
-  <si>
     <t>Review Day Part 2</t>
   </si>
   <si>
     <t>**FINAL PROJECT DUE BY 9am**</t>
-  </si>
-  <si>
-    <t>Tues, May 2</t>
   </si>
   <si>
     <t xml:space="preserve">Dangers of Early Stopping:
@@ -392,25 +301,110 @@
 </t>
   </si>
   <si>
-    <t>Wed, Apr 19</t>
-  </si>
-  <si>
-    <t>**FINAL PROJECT ROUGH DRAFTS DUE 9am** if you want feedback by Friday</t>
-  </si>
-  <si>
-    <t>Mon, Apr 24</t>
-  </si>
-  <si>
-    <t>**FINAL PROJECT ROUGH DRAFTS DUE 9am**. Feedback guaranteed by 27th.</t>
-  </si>
-  <si>
     <t>- `Stop Using Black Boxes &lt;https://arxiv.org/abs/1811.10154&gt;`_
 - `Writing to Stakeholders &lt;writing_to_stakeholders.ipynb&gt;`_
-**Optiona But Really Funl:**
+**Optional:**
 - `Contraining Artificial Stupidity &lt;https://www.youtube.com/watch?v=Z8MEFI7ZJlA&gt;`_
-**Optional But Interesting:**
 - `Black box models require trusting data too &lt;https://www.nytimes.com/2017/06/13/opinion/how-computers-are-harming-criminal-justice.html&gt;`_
+- `Why are we using Black Boxes? &lt;https://hdsr.mitpress.mit.edu/pub/f9kuryi8/release/8&gt;`_
+- `Combining explicit models and black boxes in Scientific ML &lt;https://notamonadtutorial.com/scientific-machine-learning-with-julia-the-sciml-ecosystem-b22802951c8a&gt;`_
 **FINAL PROJECT ROUGH DRAFTS DUE**</t>
+  </si>
+  <si>
+    <t>Thrs, Jan 11</t>
+  </si>
+  <si>
+    <t>Tues, Jan 16</t>
+  </si>
+  <si>
+    <t>Thrs, Jan 18</t>
+  </si>
+  <si>
+    <t>Tues, Jan 23</t>
+  </si>
+  <si>
+    <t>Thrs, Jan 25</t>
+  </si>
+  <si>
+    <t>Tues, Jan 30</t>
+  </si>
+  <si>
+    <t>Thrs, Feb 1</t>
+  </si>
+  <si>
+    <t>Tues, Feb 6</t>
+  </si>
+  <si>
+    <t>Thrs, Feb 8</t>
+  </si>
+  <si>
+    <t>Tues, Feb 13</t>
+  </si>
+  <si>
+    <t>Thrs, Feb 15</t>
+  </si>
+  <si>
+    <t>Tues, Feb 20</t>
+  </si>
+  <si>
+    <t>Thrs, Feb 22</t>
+  </si>
+  <si>
+    <t>Tues, Feb 27</t>
+  </si>
+  <si>
+    <t>Thrs, Feb 29</t>
+  </si>
+  <si>
+    <t>Tues, Mar 5</t>
+  </si>
+  <si>
+    <t>Thrs, Mar 7</t>
+  </si>
+  <si>
+    <t>Tues, Mar 12</t>
+  </si>
+  <si>
+    <t>Thrs, Mar 14</t>
+  </si>
+  <si>
+    <t>Tues, Mar 19</t>
+  </si>
+  <si>
+    <t>Thrs, Mar 21</t>
+  </si>
+  <si>
+    <t>Tues, Mar 26</t>
+  </si>
+  <si>
+    <t>Thrs, Mar 28</t>
+  </si>
+  <si>
+    <t>Tues, Apr 2</t>
+  </si>
+  <si>
+    <t>Thrs, Apr 4</t>
+  </si>
+  <si>
+    <t>Tues, Apr 9</t>
+  </si>
+  <si>
+    <t>Thrs, Apr 11</t>
+  </si>
+  <si>
+    <t>Tues, Apr 16</t>
+  </si>
+  <si>
+    <t>Interpretability
+**LAST CLASS**</t>
+  </si>
+  <si>
+    <t>- `Passive Prediction &lt;https://ds4humans.com/30_questions/20_passive_prediction_questions.html&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Causal Questions &lt;https://ds4humans.com/30_questions/30_causal_questions.html&gt;`_
+- M&amp;W, Chpt 1 - 1.1, 1.3.2 parts "The Causal Effective Catholic Schooling on Learning" and "The Causal Effective Worker Training on Earnings", 1.4
+- `How To Read &lt;how_to_read.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -843,10 +837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -868,12 +862,12 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="84">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="121">
       <c r="A2" s="9" t="s">
-        <v>15</v>
+        <v>67</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>3</v>
@@ -883,29 +877,29 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="64">
+    <row r="3" spans="1:4" ht="69">
       <c r="A3" s="9" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="34">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="35">
       <c r="A4" s="9" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>14</v>
@@ -913,332 +907,329 @@
     </row>
     <row r="5" spans="1:4" ht="119" customHeight="1">
       <c r="A5" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>45</v>
-      </c>
       <c r="C5" s="11" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="247" customHeight="1">
       <c r="A6" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>46</v>
-      </c>
       <c r="C6" s="11" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="85">
+    <row r="7" spans="1:4" ht="18">
       <c r="A7" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="34">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="18">
       <c r="A8" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="48">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="69">
       <c r="A9" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>61</v>
+        <v>74</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="76" customHeight="1">
       <c r="A10" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="141" customHeight="1">
       <c r="A11" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="72" customHeight="1">
       <c r="A12" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D12" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="35">
+      <c r="A13" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="52">
+      <c r="A14" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="120">
+      <c r="A15" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="171">
+      <c r="A16" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="52">
+      <c r="A17" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="128">
-      <c r="A13" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D13" s="6" t="s">
+    <row r="18" spans="1:4" ht="137">
+      <c r="A18" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="112">
-      <c r="A14" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D14" s="6" t="s">
+    <row r="19" spans="1:4" ht="120">
+      <c r="A19" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="128">
-      <c r="A15" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="17">
-      <c r="A16" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="17">
-      <c r="A17" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="24" customHeight="1">
       <c r="A20" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>8</v>
+        <v>85</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="178" customHeight="1">
       <c r="A21" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>13</v>
+        <v>86</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="63" customHeight="1">
       <c r="A22" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="18">
+      <c r="A23" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="1" t="s">
+    </row>
+    <row r="24" spans="1:4" ht="18">
+      <c r="A24" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="18">
+      <c r="A25" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="154">
+      <c r="A26" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="18">
+      <c r="A27" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="204">
-      <c r="A23" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="141">
-      <c r="A24" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="34">
-      <c r="A25" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="17">
-      <c r="A26" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D26" s="7"/>
-    </row>
-    <row r="27" spans="1:4" ht="17">
-      <c r="A27" s="9" t="s">
+    <row r="28" spans="1:4" ht="205">
+      <c r="A28" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="142">
+      <c r="A29" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D27" s="6"/>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="222">
-      <c r="A29" s="9" t="s">
+    </row>
+    <row r="30" spans="1:4" ht="35">
+      <c r="A30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="18">
+      <c r="A31" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="112">
-      <c r="A33" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>92</v>
+      <c r="D31" s="7"/>
+    </row>
+    <row r="32" spans="1:4" ht="17">
+      <c r="B32" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="6"/>
+    </row>
+    <row r="33" spans="2:3" ht="17">
+      <c r="B33" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="C33" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" ht="221">
+      <c r="B34" s="1" t="s">
         <v>95</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" ht="17">
+      <c r="C35" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" ht="136">
+      <c r="B36" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update schedule with exercise
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A8AAA81A-F0A1-5241-8CC0-0BB24684215B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1334E115-2207-2944-8942-2E83CD0B8793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6460" yWindow="2520" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="76">
   <si>
     <t>Date</t>
   </si>
@@ -300,6 +300,9 @@
   </si>
   <si>
     <t>- `Acme Proposal &lt;exercises/exercise_first_class_capstone_proposal.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Stakeholder Management &lt;exercise_stakeholder_management.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -1149,8 +1152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1211,6 +1214,9 @@
       <c r="C4" s="2" t="s">
         <v>71</v>
       </c>
+      <c r="D4" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="67" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">

</xml_diff>

<commit_message>
update exercise and schedule
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A930CE8D-18CD-A84E-B9F1-6B052FE6D61F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED8A7E3-5B01-E246-8E2A-8C2D054CE414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6460" yWindow="2520" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1153,7 +1153,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
update exploratory and public data
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA163E17-26EC-6844-A6B1-7768D36A1715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FFCE8A9-DE30-B54F-B652-ACCF59BAF3A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6460" yWindow="2520" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,9 +68,6 @@
     <t>Proscriptive v. Descriptive Questions</t>
   </si>
   <si>
-    <t>- `Descriptive versus Proscriptive Questions &lt;https://ds4humans.com/30_questions/05_descriptive_v_proscriptive.html&gt;`_</t>
-  </si>
-  <si>
     <t>Thrs, Jan 25</t>
   </si>
   <si>
@@ -303,6 +300,9 @@
 - `Using Exploratory Questions &lt;https://ds4humans.com/30_questions/10_using_exploratory_questions.html&gt;`_
 - `Answering Exploratory Questions &lt;https://ds4humans.com/30_questions/15_answering_exploratory_questions.html&gt;`_
 - `Internal v. External Validity &lt;https://ds4humans.com/30_questions/17_exploratory_questions_internal_external.html&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Descriptive versus Prescriptive Questions &lt;https://ds4humans.com/30_questions/05_descriptive_v_prescriptive.html&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -1153,7 +1153,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1173,7 +1173,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1184,10 +1184,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="102" x14ac:dyDescent="0.2">
@@ -1198,10 +1198,10 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="136" x14ac:dyDescent="0.2">
@@ -1212,10 +1212,10 @@
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="67" customHeight="1" x14ac:dyDescent="0.2">
@@ -1225,262 +1225,262 @@
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
-        <v>11</v>
+      <c r="C5" s="3" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="115" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
       <c r="C6" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4" ht="65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
       <c r="C8" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="153" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
       <c r="C9" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
       <c r="C10" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
         <v>24</v>
       </c>
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
       <c r="C12" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="102" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="153" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
         <v>36</v>
-      </c>
-      <c r="B19" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="187" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" t="s">
         <v>49</v>
-      </c>
-      <c r="C27" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="136" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" t="s">
         <v>55</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>